<commit_message>
update Cvb Tabel - exe file doesn't work yet
</commit_message>
<xml_diff>
--- a/CVB-Tabel.xlsx
+++ b/CVB-Tabel.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghanm\Documents\ILVO Projects\Drupal RekeningTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E5C1F0-BA2D-423D-994E-D027B0441197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2291DD91-26B9-480E-824B-E8E252EEF548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -207,21 +218,6 @@
     <t xml:space="preserve">Palmpitschroot, RC &gt; 190 g/kg   </t>
   </si>
   <si>
-    <t>Raapzaad</t>
-  </si>
-  <si>
-    <t>Raapzaadschilfers</t>
-  </si>
-  <si>
-    <t>Raapzaadschroot bestendig, Mervobest</t>
-  </si>
-  <si>
-    <t>Raapzaadschroot, RE &lt; 370 g/kg</t>
-  </si>
-  <si>
-    <t>Raapzaadschroot, RE &gt; 370 g/kg</t>
-  </si>
-  <si>
     <t>Rogge</t>
   </si>
   <si>
@@ -327,9 +323,6 @@
     <t>Vet/olie, Palmpitolie, chem. geraf.</t>
   </si>
   <si>
-    <t>Vet/olie, Raapzaadolie</t>
-  </si>
-  <si>
     <t>Vet/olie, Sojaolie</t>
   </si>
   <si>
@@ -492,9 +485,6 @@
     <t>Luzerne, vers</t>
   </si>
   <si>
-    <t>Raapzaadstro</t>
-  </si>
-  <si>
     <t>Roggestro</t>
   </si>
   <si>
@@ -607,6 +597,27 @@
   </si>
   <si>
     <t>Tarwegistconcentraat, RE 275 - 325 g/kg DS</t>
+  </si>
+  <si>
+    <t>koolzaad</t>
+  </si>
+  <si>
+    <t>koolzaadschilfers</t>
+  </si>
+  <si>
+    <t>koolzaadschroot bestendig, Mervobest</t>
+  </si>
+  <si>
+    <t>koolzaadschroot, RE &lt; 370 g/kg</t>
+  </si>
+  <si>
+    <t>koolzaadschroot, RE &gt; 370 g/kg</t>
+  </si>
+  <si>
+    <t>Vet/olie, koolzaadolie</t>
+  </si>
+  <si>
+    <t>koolzaadstro</t>
   </si>
 </sst>
 </file>
@@ -941,7 +952,7 @@
   <dimension ref="A1:G184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2143,7 +2154,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>187</v>
       </c>
       <c r="B53" t="s">
         <v>8</v>
@@ -2166,7 +2177,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>61</v>
+        <v>188</v>
       </c>
       <c r="B54" t="s">
         <v>8</v>
@@ -2189,7 +2200,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>189</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
@@ -2212,7 +2223,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>190</v>
       </c>
       <c r="B56" t="s">
         <v>8</v>
@@ -2235,7 +2246,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>64</v>
+        <v>191</v>
       </c>
       <c r="B57" t="s">
         <v>8</v>
@@ -2258,7 +2269,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
         <v>8</v>
@@ -2281,7 +2292,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B59" t="s">
         <v>8</v>
@@ -2304,7 +2315,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B60" t="s">
         <v>8</v>
@@ -2327,7 +2338,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B61" t="s">
         <v>8</v>
@@ -2350,7 +2361,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
         <v>8</v>
@@ -2373,7 +2384,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
@@ -2396,7 +2407,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B64" t="s">
         <v>8</v>
@@ -2419,7 +2430,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B65" t="s">
         <v>8</v>
@@ -2442,7 +2453,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B66" t="s">
         <v>8</v>
@@ -2465,7 +2476,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B67" t="s">
         <v>8</v>
@@ -2488,7 +2499,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B68" t="s">
         <v>8</v>
@@ -2511,7 +2522,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B69" t="s">
         <v>8</v>
@@ -2534,7 +2545,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B70" t="s">
         <v>8</v>
@@ -2557,7 +2568,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B71" t="s">
         <v>8</v>
@@ -2580,7 +2591,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B72" t="s">
         <v>8</v>
@@ -2603,7 +2614,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B73" t="s">
         <v>8</v>
@@ -2626,7 +2637,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B74" t="s">
         <v>8</v>
@@ -2643,7 +2654,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B75" t="s">
         <v>8</v>
@@ -2666,7 +2677,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B76" t="s">
         <v>8</v>
@@ -2689,7 +2700,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B77" t="s">
         <v>8</v>
@@ -2712,7 +2723,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B78" t="s">
         <v>8</v>
@@ -2735,7 +2746,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B79" t="s">
         <v>8</v>
@@ -2758,7 +2769,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B80" t="s">
         <v>8</v>
@@ -2781,7 +2792,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B81" t="s">
         <v>8</v>
@@ -2804,7 +2815,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B82" t="s">
         <v>8</v>
@@ -2827,7 +2838,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B83" t="s">
         <v>8</v>
@@ -2850,7 +2861,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B84" t="s">
         <v>8</v>
@@ -2873,7 +2884,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B85" t="s">
         <v>8</v>
@@ -2896,7 +2907,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B86" t="s">
         <v>8</v>
@@ -2919,7 +2930,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B87" t="s">
         <v>8</v>
@@ -2942,7 +2953,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B88" t="s">
         <v>8</v>
@@ -2965,7 +2976,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B89" t="s">
         <v>8</v>
@@ -2988,7 +2999,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B90" t="s">
         <v>8</v>
@@ -3011,7 +3022,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B91" t="s">
         <v>8</v>
@@ -3034,7 +3045,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B92" t="s">
         <v>8</v>
@@ -3057,7 +3068,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>100</v>
+        <v>192</v>
       </c>
       <c r="B93" t="s">
         <v>8</v>
@@ -3080,7 +3091,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B94" t="s">
         <v>8</v>
@@ -3103,7 +3114,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B95" t="s">
         <v>8</v>
@@ -3126,7 +3137,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B96" t="s">
         <v>8</v>
@@ -3149,7 +3160,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B97" t="s">
         <v>8</v>
@@ -3172,7 +3183,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B98" t="s">
         <v>8</v>
@@ -3195,7 +3206,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B99" t="s">
         <v>8</v>
@@ -3218,7 +3229,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B100" t="s">
         <v>8</v>
@@ -3241,10 +3252,10 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C101" t="s">
         <v>9</v>
@@ -3264,10 +3275,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C102" t="s">
         <v>9</v>
@@ -3287,10 +3298,10 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C103" t="s">
         <v>9</v>
@@ -3310,10 +3321,10 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C104" t="s">
         <v>9</v>
@@ -3333,10 +3344,10 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C105" t="s">
         <v>9</v>
@@ -3356,10 +3367,10 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C106" t="s">
         <v>9</v>
@@ -3379,10 +3390,10 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C107" t="s">
         <v>9</v>
@@ -3402,10 +3413,10 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C108" t="s">
         <v>9</v>
@@ -3425,10 +3436,10 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C109" t="s">
         <v>9</v>
@@ -3448,10 +3459,10 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C110" t="s">
         <v>9</v>
@@ -3471,10 +3482,10 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C111" t="s">
         <v>9</v>
@@ -3494,10 +3505,10 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C112" t="s">
         <v>9</v>
@@ -3517,10 +3528,10 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C113" t="s">
         <v>9</v>
@@ -3540,10 +3551,10 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C114" t="s">
         <v>9</v>
@@ -3563,10 +3574,10 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C115" t="s">
         <v>9</v>
@@ -3586,10 +3597,10 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C116" t="s">
         <v>9</v>
@@ -3609,10 +3620,10 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C117" t="s">
         <v>9</v>
@@ -3632,10 +3643,10 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B118" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C118" t="s">
         <v>9</v>
@@ -3655,10 +3666,10 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C119" t="s">
         <v>9</v>
@@ -3678,10 +3689,10 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C120" t="s">
         <v>9</v>
@@ -3701,10 +3712,10 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C121" t="s">
         <v>9</v>
@@ -3724,10 +3735,10 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C122" t="s">
         <v>9</v>
@@ -3747,10 +3758,10 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C123" t="s">
         <v>9</v>
@@ -3770,10 +3781,10 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B124" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C124" t="s">
         <v>9</v>
@@ -3793,10 +3804,10 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B125" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C125" t="s">
         <v>9</v>
@@ -3816,10 +3827,10 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B126" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C126" t="s">
         <v>9</v>
@@ -3839,10 +3850,10 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B127" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C127" t="s">
         <v>9</v>
@@ -3862,10 +3873,10 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B128" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C128" t="s">
         <v>9</v>
@@ -3885,10 +3896,10 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C129" t="s">
         <v>9</v>
@@ -3908,10 +3919,10 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B130" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C130" t="s">
         <v>9</v>
@@ -3931,10 +3942,10 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B131" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C131" t="s">
         <v>9</v>
@@ -3954,10 +3965,10 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B132" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C132" t="s">
         <v>9</v>
@@ -3977,10 +3988,10 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B133" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C133" t="s">
         <v>9</v>
@@ -4000,10 +4011,10 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B134" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C134" t="s">
         <v>9</v>
@@ -4023,10 +4034,10 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B135" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C135" t="s">
         <v>9</v>
@@ -4046,10 +4057,10 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B136" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C136" t="s">
         <v>9</v>
@@ -4069,10 +4080,10 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B137" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C137" t="s">
         <v>9</v>
@@ -4092,10 +4103,10 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B138" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C138" t="s">
         <v>9</v>
@@ -4115,10 +4126,10 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B139" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C139" t="s">
         <v>9</v>
@@ -4138,10 +4149,10 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B140" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C140" t="s">
         <v>9</v>
@@ -4161,10 +4172,10 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B141" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C141" t="s">
         <v>9</v>
@@ -4184,10 +4195,10 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B142" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C142" t="s">
         <v>9</v>
@@ -4207,10 +4218,10 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B143" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C143" t="s">
         <v>9</v>
@@ -4230,10 +4241,10 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B144" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C144" t="s">
         <v>9</v>
@@ -4253,10 +4264,10 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B145" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C145" t="s">
         <v>9</v>
@@ -4276,10 +4287,10 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B146" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C146" t="s">
         <v>9</v>
@@ -4299,10 +4310,10 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>155</v>
+        <v>193</v>
       </c>
       <c r="B147" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C147" t="s">
         <v>9</v>
@@ -4322,10 +4333,10 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B148" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C148" t="s">
         <v>9</v>
@@ -4345,10 +4356,10 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B149" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C149" t="s">
         <v>9</v>
@@ -4368,10 +4379,10 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B150" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C150" t="s">
         <v>9</v>
@@ -4391,10 +4402,10 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B151" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C151" t="s">
         <v>9</v>
@@ -4408,10 +4419,10 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B152" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C152" t="s">
         <v>9</v>
@@ -4431,10 +4442,10 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B153" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C153" t="s">
         <v>9</v>
@@ -4454,10 +4465,10 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B154" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C154" t="s">
         <v>9</v>
@@ -4477,10 +4488,10 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B155" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C155" t="s">
         <v>9</v>
@@ -4500,10 +4511,10 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B156" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C156" t="s">
         <v>9</v>
@@ -4523,10 +4534,10 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B157" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C157" t="s">
         <v>9</v>
@@ -4546,10 +4557,10 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B158" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C158" t="s">
         <v>9</v>
@@ -4569,10 +4580,10 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B159" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C159" t="s">
         <v>9</v>
@@ -4592,10 +4603,10 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B160" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C160" t="s">
         <v>9</v>
@@ -4615,10 +4626,10 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B161" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C161" t="s">
         <v>9</v>
@@ -4638,10 +4649,10 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B162" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C162" t="s">
         <v>9</v>
@@ -4661,10 +4672,10 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B163" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C163" t="s">
         <v>9</v>
@@ -4684,10 +4695,10 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B164" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C164" t="s">
         <v>9</v>
@@ -4707,10 +4718,10 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B165" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C165" t="s">
         <v>9</v>
@@ -4730,10 +4741,10 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B166" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C166" t="s">
         <v>9</v>
@@ -4753,10 +4764,10 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B167" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C167" t="s">
         <v>9</v>
@@ -4776,10 +4787,10 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B168" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C168" t="s">
         <v>9</v>
@@ -4799,10 +4810,10 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B169" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C169" t="s">
         <v>9</v>
@@ -4822,10 +4833,10 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B170" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C170" t="s">
         <v>9</v>
@@ -4845,10 +4856,10 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B171" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C171" t="s">
         <v>9</v>
@@ -4868,10 +4879,10 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B172" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C172" t="s">
         <v>9</v>
@@ -4891,10 +4902,10 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B173" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C173" t="s">
         <v>9</v>
@@ -4914,10 +4925,10 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B174" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C174" t="s">
         <v>9</v>
@@ -4937,10 +4948,10 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B175" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C175" t="s">
         <v>9</v>
@@ -4960,10 +4971,10 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B176" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C176" t="s">
         <v>9</v>
@@ -4983,10 +4994,10 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B177" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C177" t="s">
         <v>9</v>
@@ -5006,10 +5017,10 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B178" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C178" t="s">
         <v>9</v>
@@ -5023,10 +5034,10 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B179" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C179" t="s">
         <v>9</v>
@@ -5046,10 +5057,10 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B180" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C180" t="s">
         <v>9</v>
@@ -5069,10 +5080,10 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B181" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C181" t="s">
         <v>9</v>
@@ -5086,10 +5097,10 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B182" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C182" t="s">
         <v>9</v>
@@ -5109,10 +5120,10 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B183" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C183" t="s">
         <v>9</v>
@@ -5132,10 +5143,10 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B184" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C184" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
feat(export): allow export without real price and handle missing feed values
- Enabled Excel and PDF export even when no real price is entered
- Excluded feed items that only contain DS (no DVE, VEM, or VEVI values)
- Retained items missing only DVE by setting DVE = 0
- Applied consistent filtering logic for both Excel and PDF exports
</commit_message>
<xml_diff>
--- a/CVB-Tabel.xlsx
+++ b/CVB-Tabel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghanm\Documents\ILVO Projects\Drupal RekeningTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2291DD91-26B9-480E-824B-E8E252EEF548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B046EE03-506B-4B97-B61E-2A295D7901CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -668,7 +668,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -952,14 +952,15 @@
   <dimension ref="A1:G184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
-    <col min="3" max="7" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="7" width="11.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,16 +973,16 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -998,13 +999,13 @@
       <c r="D2" s="2">
         <v>962.44</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>80.068979999999996</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>1670.7538</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>1887.93136</v>
       </c>
     </row>
@@ -1021,13 +1022,13 @@
       <c r="D3" s="2">
         <v>915.38</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>151.94931</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>896.93709000000001</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>898.56206999999995</v>
       </c>
     </row>
@@ -1044,13 +1045,13 @@
       <c r="D4" s="2">
         <v>893.38</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>100.5587</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>1043.8556799999999</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>1129.8622700000001</v>
       </c>
     </row>
@@ -1067,13 +1068,13 @@
       <c r="D5" s="2">
         <v>911.56</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>103.21064</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>1033.5328099999999</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>1123.17669</v>
       </c>
     </row>
@@ -1090,13 +1091,13 @@
       <c r="D6" s="2">
         <v>900.76</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>103.22696999999999</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>1034.93129</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>1120.1067399999999</v>
       </c>
     </row>
@@ -1113,13 +1114,13 @@
       <c r="D7" s="2">
         <v>905.75</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>103.45577</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>1030.1044099999999</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>1118.42425</v>
       </c>
     </row>
@@ -1136,13 +1137,13 @@
       <c r="D8" s="2">
         <v>862.42</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>157.22218000000001</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>1133.2436399999999</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>1233.32494</v>
       </c>
     </row>
@@ -1159,13 +1160,13 @@
       <c r="D9" s="2">
         <v>896.64</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>98.192490000000006</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>1012.50109</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>1087.8385000000001</v>
       </c>
     </row>
@@ -1182,13 +1183,13 @@
       <c r="D10" s="2">
         <v>912.47</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>87.001040000000003</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>1061.5995499999999</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>1157.8351</v>
       </c>
     </row>
@@ -1205,13 +1206,13 @@
       <c r="D11" s="2">
         <v>903.05</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>219.6146</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>1308.47453</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>1422.79548</v>
       </c>
     </row>
@@ -1228,13 +1229,13 @@
       <c r="D12" s="2">
         <v>915.95</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>220.49800999999999</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>1168.81331</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>1250.7056600000001</v>
       </c>
     </row>
@@ -1251,13 +1252,13 @@
       <c r="D13" s="2">
         <v>866.43</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>121.30409</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>1180.75172</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <v>1295.67147</v>
       </c>
     </row>
@@ -1274,13 +1275,13 @@
       <c r="D14" s="2">
         <v>873.39</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>116.18989999999999</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>1122.4374499999999</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <v>1225.41085</v>
       </c>
     </row>
@@ -1297,13 +1298,13 @@
       <c r="D15" s="2">
         <v>885.98</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>68.651169999999993</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>850.53975000000003</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="2">
         <v>863.34649000000002</v>
       </c>
     </row>
@@ -1320,13 +1321,13 @@
       <c r="D16" s="2">
         <v>878.53</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>81.365080000000006</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <v>1042.0897299999999</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
         <v>1106.8208099999999</v>
       </c>
     </row>
@@ -1343,13 +1344,13 @@
       <c r="D17" s="2">
         <v>886</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>71.176329999999993</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <v>1019.24833</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="2">
         <v>1076.40571</v>
       </c>
     </row>
@@ -1366,13 +1367,13 @@
       <c r="D18" s="2">
         <v>895.87</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>131.25913</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <v>852.18289000000004</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="2">
         <v>842.15457000000004</v>
       </c>
     </row>
@@ -1389,13 +1390,13 @@
       <c r="D19" s="2">
         <v>945</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>102.02088999999999</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>846.47573999999997</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="2">
         <v>834.44183999999996</v>
       </c>
     </row>
@@ -1412,13 +1413,13 @@
       <c r="D20" s="2">
         <v>897.69</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>155.25675000000001</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>920.25359000000003</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <v>923.96870000000001</v>
       </c>
     </row>
@@ -1435,13 +1436,13 @@
       <c r="D21" s="2">
         <v>907.19</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>174.45741000000001</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>1174.7155600000001</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="2">
         <v>1269.44751</v>
       </c>
     </row>
@@ -1458,13 +1459,13 @@
       <c r="D22" s="2">
         <v>941.34</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>170.69685000000001</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>1264.7696699999999</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="2">
         <v>1377.74693</v>
       </c>
     </row>
@@ -1481,13 +1482,13 @@
       <c r="D23" s="2">
         <v>909.96</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>191.60911999999999</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>993.64426000000003</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="2">
         <v>1046.6861200000001</v>
       </c>
     </row>
@@ -1504,13 +1505,13 @@
       <c r="D24" s="2">
         <v>921.64</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>72.593310000000002</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>1930.23395</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="2">
         <v>2175.9142999999999</v>
       </c>
     </row>
@@ -1527,13 +1528,13 @@
       <c r="D25" s="2">
         <v>922.34</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>170.05787000000001</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <v>1123.5702200000001</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="2">
         <v>1187.29981</v>
       </c>
     </row>
@@ -1550,13 +1551,13 @@
       <c r="D26" s="2">
         <v>871.95</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>172.70079999999999</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <v>991.20820000000003</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="2">
         <v>1026.8215499999999</v>
       </c>
     </row>
@@ -1573,13 +1574,13 @@
       <c r="D27" s="2">
         <v>895.45</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>138.78116</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <v>1267.61337</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="2">
         <v>1378.79988</v>
       </c>
     </row>
@@ -1596,13 +1597,13 @@
       <c r="D28" s="2">
         <v>878.13</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>155.03582</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="2">
         <v>1253.5342900000001</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="2">
         <v>1357.70219</v>
       </c>
     </row>
@@ -1619,13 +1620,13 @@
       <c r="D29" s="2">
         <v>918.07</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <v>50.546500000000002</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="2">
         <v>672.45754999999997</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="2">
         <v>640.52350000000001</v>
       </c>
     </row>
@@ -1642,13 +1643,13 @@
       <c r="D30" s="2">
         <v>906.36</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <v>92.593869999999995</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="2">
         <v>768.83529999999996</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="2">
         <v>760.32857999999999</v>
       </c>
     </row>
@@ -1665,13 +1666,13 @@
       <c r="D31" s="2">
         <v>912.72</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <v>73.604879999999994</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="2">
         <v>681.13905999999997</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="2">
         <v>649.14553000000001</v>
       </c>
     </row>
@@ -1688,13 +1689,13 @@
       <c r="D32" s="2">
         <v>914.21</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="2">
         <v>79.818899999999999</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="2">
         <v>692.72222999999997</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32" s="2">
         <v>663.63991999999996</v>
       </c>
     </row>
@@ -1711,13 +1712,13 @@
       <c r="D33" s="2">
         <v>863.05</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="2">
         <v>113.35342</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="2">
         <v>1257.0975800000001</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G33" s="2">
         <v>1402.7394400000001</v>
       </c>
     </row>
@@ -1734,13 +1735,13 @@
       <c r="D34" s="2">
         <v>875.99</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="2">
         <v>152.37313</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="2">
         <v>1278.47272</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="2">
         <v>1431.44218</v>
       </c>
     </row>
@@ -1757,13 +1758,13 @@
       <c r="D35" s="2">
         <v>899.49</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="2">
         <v>499.24790999999999</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="2">
         <v>1348.92616</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35" s="2">
         <v>1454.9837299999999</v>
       </c>
     </row>
@@ -1780,13 +1781,13 @@
       <c r="D36" s="2">
         <v>881.56</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="2">
         <v>106.55336</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="2">
         <v>1084.27712</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36" s="2">
         <v>1166.1889100000001</v>
       </c>
     </row>
@@ -1803,13 +1804,13 @@
       <c r="D37" s="2">
         <v>889.45</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="2">
         <v>100.73742</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="2">
         <v>1080.2978700000001</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37" s="2">
         <v>1154.4858400000001</v>
       </c>
     </row>
@@ -1826,13 +1827,13 @@
       <c r="D38" s="2">
         <v>892.59</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="2">
         <v>101.93591000000001</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="2">
         <v>1084.52684</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38" s="2">
         <v>1163.23155</v>
       </c>
     </row>
@@ -1849,13 +1850,13 @@
       <c r="D39" s="2">
         <v>876.41</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="2">
         <v>179.82432</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="2">
         <v>1063.3259399999999</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39" s="2">
         <v>1126.50018</v>
       </c>
     </row>
@@ -1872,13 +1873,13 @@
       <c r="D40" s="2">
         <v>875.49</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="2">
         <v>122.63415999999999</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="2">
         <v>1247.32349</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G40" s="2">
         <v>1398.08932</v>
       </c>
     </row>
@@ -1895,13 +1896,13 @@
       <c r="D41" s="2">
         <v>878.69</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="2">
         <v>107.88104</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="2">
         <v>1260.7970800000001</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="2">
         <v>1398.59824</v>
       </c>
     </row>
@@ -1918,13 +1919,13 @@
       <c r="D42" s="2">
         <v>867.2</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="2">
         <v>118.53259</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="2">
         <v>1241.1402700000001</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42" s="2">
         <v>1381.3437300000001</v>
       </c>
     </row>
@@ -1941,13 +1942,13 @@
       <c r="D43" s="2">
         <v>787.33</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="2">
         <v>76.254499999999993</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43" s="2">
         <v>1022.57748</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G43" s="2">
         <v>1129.9573800000001</v>
       </c>
     </row>
@@ -1964,13 +1965,13 @@
       <c r="D44" s="2">
         <v>917.84</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="2">
         <v>69.68741</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44" s="2">
         <v>784.07934</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G44" s="2">
         <v>774.01284999999996</v>
       </c>
     </row>
@@ -1987,13 +1988,13 @@
       <c r="D45" s="2">
         <v>914.19</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="2">
         <v>82.500339999999994</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45" s="2">
         <v>938.60807</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G45" s="2">
         <v>973.3913</v>
       </c>
     </row>
@@ -2010,13 +2011,13 @@
       <c r="D46" s="2">
         <v>868.54</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="2">
         <v>131.14133000000001</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46" s="2">
         <v>1172.76567</v>
       </c>
-      <c r="G46" s="3">
+      <c r="G46" s="2">
         <v>1277.0692899999999</v>
       </c>
     </row>
@@ -2033,13 +2034,13 @@
       <c r="D47" s="2">
         <v>867.09</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="2">
         <v>132.94291000000001</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47" s="2">
         <v>1167.02972</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G47" s="2">
         <v>1268.3821</v>
       </c>
     </row>
@@ -2056,13 +2057,13 @@
       <c r="D48" s="2">
         <v>918.61</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="2">
         <v>127.60527</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F48" s="2">
         <v>1136.6498899999999</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G48" s="2">
         <v>1214.4941899999999</v>
       </c>
     </row>
@@ -2079,13 +2080,13 @@
       <c r="D49" s="2">
         <v>927.13</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="2">
         <v>118.64261999999999</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F49" s="2">
         <v>1074.7140099999999</v>
       </c>
-      <c r="G49" s="3">
+      <c r="G49" s="2">
         <v>1131.7953199999999</v>
       </c>
     </row>
@@ -2102,9 +2103,15 @@
       <c r="D50" s="2">
         <v>879.56</v>
       </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
+      <c r="E50" s="2">
+        <v>0</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0</v>
+      </c>
+      <c r="G50" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -2119,13 +2126,13 @@
       <c r="D51" s="2">
         <v>892.77</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51" s="2">
         <v>134.25316000000001</v>
       </c>
-      <c r="F51" s="3">
+      <c r="F51" s="2">
         <v>975.24495000000002</v>
       </c>
-      <c r="G51" s="3">
+      <c r="G51" s="2">
         <v>1017.70763</v>
       </c>
     </row>
@@ -2142,13 +2149,13 @@
       <c r="D52" s="2">
         <v>875.52</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="2">
         <v>125.20237</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F52" s="2">
         <v>869.51274000000001</v>
       </c>
-      <c r="G52" s="3">
+      <c r="G52" s="2">
         <v>880.97877000000005</v>
       </c>
     </row>
@@ -2165,13 +2172,13 @@
       <c r="D53" s="2">
         <v>924.67</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53" s="2">
         <v>37.284390000000002</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F53" s="2">
         <v>2028.4947099999999</v>
       </c>
-      <c r="G53" s="3">
+      <c r="G53" s="2">
         <v>2304.1664000000001</v>
       </c>
     </row>
@@ -2188,13 +2195,13 @@
       <c r="D54" s="2">
         <v>902.31</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E54" s="2">
         <v>131.13724999999999</v>
       </c>
-      <c r="F54" s="3">
+      <c r="F54" s="2">
         <v>1169.60465</v>
       </c>
-      <c r="G54" s="3">
+      <c r="G54" s="2">
         <v>1243.39733</v>
       </c>
     </row>
@@ -2211,13 +2218,13 @@
       <c r="D55" s="2">
         <v>877.02</v>
       </c>
-      <c r="E55" s="3">
+      <c r="E55" s="2">
         <v>295.27890000000002</v>
       </c>
-      <c r="F55" s="3">
+      <c r="F55" s="2">
         <v>944.27094999999997</v>
       </c>
-      <c r="G55" s="3">
+      <c r="G55" s="2">
         <v>966.06867</v>
       </c>
     </row>
@@ -2234,13 +2241,13 @@
       <c r="D56" s="2">
         <v>881.6</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E56" s="2">
         <v>144.71459999999999</v>
       </c>
-      <c r="F56" s="3">
+      <c r="F56" s="2">
         <v>972.55381</v>
       </c>
-      <c r="G56" s="3">
+      <c r="G56" s="2">
         <v>1004.14373</v>
       </c>
     </row>
@@ -2257,13 +2264,13 @@
       <c r="D57" s="2">
         <v>896.92</v>
       </c>
-      <c r="E57" s="3">
+      <c r="E57" s="2">
         <v>157.26173</v>
       </c>
-      <c r="F57" s="3">
+      <c r="F57" s="2">
         <v>950.41858999999999</v>
       </c>
-      <c r="G57" s="3">
+      <c r="G57" s="2">
         <v>977.3827</v>
       </c>
     </row>
@@ -2280,13 +2287,13 @@
       <c r="D58" s="2">
         <v>869.5</v>
       </c>
-      <c r="E58" s="3">
+      <c r="E58" s="2">
         <v>111.05419000000001</v>
       </c>
-      <c r="F58" s="3">
+      <c r="F58" s="2">
         <v>1158.24134</v>
       </c>
-      <c r="G58" s="3">
+      <c r="G58" s="2">
         <v>1276.77638</v>
       </c>
     </row>
@@ -2303,13 +2310,13 @@
       <c r="D59" s="2">
         <v>898.9</v>
       </c>
-      <c r="E59" s="3">
+      <c r="E59" s="2">
         <v>118.97512999999999</v>
       </c>
-      <c r="F59" s="3">
+      <c r="F59" s="2">
         <v>1585.3824400000001</v>
       </c>
-      <c r="G59" s="3">
+      <c r="G59" s="2">
         <v>1763.18237</v>
       </c>
     </row>
@@ -2326,13 +2333,13 @@
       <c r="D60" s="2">
         <v>898.9</v>
       </c>
-      <c r="E60" s="3">
+      <c r="E60" s="2">
         <v>173.58584999999999</v>
       </c>
-      <c r="F60" s="3">
+      <c r="F60" s="2">
         <v>1585.39041</v>
       </c>
-      <c r="G60" s="3">
+      <c r="G60" s="2">
         <v>1763.1896300000001</v>
       </c>
     </row>
@@ -2349,13 +2356,13 @@
       <c r="D61" s="2">
         <v>883.03</v>
       </c>
-      <c r="E61" s="3">
+      <c r="E61" s="2">
         <v>89.994929999999997</v>
       </c>
-      <c r="F61" s="3">
+      <c r="F61" s="2">
         <v>1058.2932499999999</v>
       </c>
-      <c r="G61" s="3">
+      <c r="G61" s="2">
         <v>1123.3379199999999</v>
       </c>
     </row>
@@ -2372,13 +2379,13 @@
       <c r="D62" s="2">
         <v>886.79</v>
       </c>
-      <c r="E62" s="3">
+      <c r="E62" s="2">
         <v>80.40634</v>
       </c>
-      <c r="F62" s="3">
+      <c r="F62" s="2">
         <v>1003.38276</v>
       </c>
-      <c r="G62" s="3">
+      <c r="G62" s="2">
         <v>1053.6854800000001</v>
       </c>
     </row>
@@ -2395,13 +2402,13 @@
       <c r="D63" s="2">
         <v>886.07</v>
       </c>
-      <c r="E63" s="3">
+      <c r="E63" s="2">
         <v>81.533680000000004</v>
       </c>
-      <c r="F63" s="3">
+      <c r="F63" s="2">
         <v>1020.99271</v>
       </c>
-      <c r="G63" s="3">
+      <c r="G63" s="2">
         <v>1076.0888199999999</v>
       </c>
     </row>
@@ -2418,13 +2425,13 @@
       <c r="D64" s="2">
         <v>872</v>
       </c>
-      <c r="E64" s="3">
+      <c r="E64" s="2">
         <v>435.53834000000001</v>
       </c>
-      <c r="F64" s="3">
+      <c r="F64" s="2">
         <v>1136.45886</v>
       </c>
-      <c r="G64" s="3">
+      <c r="G64" s="2">
         <v>1213.64491</v>
       </c>
     </row>
@@ -2441,13 +2448,13 @@
       <c r="D65" s="2">
         <v>873.27</v>
       </c>
-      <c r="E65" s="3">
+      <c r="E65" s="2">
         <v>424.35309000000001</v>
       </c>
-      <c r="F65" s="3">
+      <c r="F65" s="2">
         <v>1139.27071</v>
       </c>
-      <c r="G65" s="3">
+      <c r="G65" s="2">
         <v>1215.7613899999999</v>
       </c>
     </row>
@@ -2464,13 +2471,13 @@
       <c r="D66" s="2">
         <v>881.51</v>
       </c>
-      <c r="E66" s="3">
+      <c r="E66" s="2">
         <v>269.77168</v>
       </c>
-      <c r="F66" s="3">
+      <c r="F66" s="2">
         <v>1152.06258</v>
       </c>
-      <c r="G66" s="3">
+      <c r="G66" s="2">
         <v>1235.71163</v>
       </c>
     </row>
@@ -2487,13 +2494,13 @@
       <c r="D67" s="2">
         <v>878.07</v>
       </c>
-      <c r="E67" s="3">
+      <c r="E67" s="2">
         <v>279.47091999999998</v>
       </c>
-      <c r="F67" s="3">
+      <c r="F67" s="2">
         <v>1153.73552</v>
       </c>
-      <c r="G67" s="3">
+      <c r="G67" s="2">
         <v>1235.4047499999999</v>
       </c>
     </row>
@@ -2510,13 +2517,13 @@
       <c r="D68" s="2">
         <v>877.54</v>
       </c>
-      <c r="E68" s="3">
+      <c r="E68" s="2">
         <v>246.25176999999999</v>
       </c>
-      <c r="F68" s="3">
+      <c r="F68" s="2">
         <v>1138.65851</v>
       </c>
-      <c r="G68" s="3">
+      <c r="G68" s="2">
         <v>1220.1039499999999</v>
       </c>
     </row>
@@ -2533,13 +2540,13 @@
       <c r="D69" s="2">
         <v>879.76</v>
       </c>
-      <c r="E69" s="3">
+      <c r="E69" s="2">
         <v>253.47504000000001</v>
       </c>
-      <c r="F69" s="3">
+      <c r="F69" s="2">
         <v>1146.0111899999999</v>
       </c>
-      <c r="G69" s="3">
+      <c r="G69" s="2">
         <v>1228.6584</v>
       </c>
     </row>
@@ -2556,13 +2563,13 @@
       <c r="D70" s="2">
         <v>877.34</v>
       </c>
-      <c r="E70" s="3">
+      <c r="E70" s="2">
         <v>268.85194999999999</v>
       </c>
-      <c r="F70" s="3">
+      <c r="F70" s="2">
         <v>1153.9401399999999</v>
       </c>
-      <c r="G70" s="3">
+      <c r="G70" s="2">
         <v>1236.3154</v>
       </c>
     </row>
@@ -2579,13 +2586,13 @@
       <c r="D71" s="2">
         <v>871.58</v>
       </c>
-      <c r="E71" s="3">
+      <c r="E71" s="2">
         <v>103.04266</v>
       </c>
-      <c r="F71" s="3">
+      <c r="F71" s="2">
         <v>1156.9828500000001</v>
       </c>
-      <c r="G71" s="3">
+      <c r="G71" s="2">
         <v>1270.1314199999999</v>
       </c>
     </row>
@@ -2602,13 +2609,13 @@
       <c r="D72" s="2">
         <v>866.55</v>
       </c>
-      <c r="E72" s="3">
+      <c r="E72" s="2">
         <v>114.29871</v>
       </c>
-      <c r="F72" s="3">
+      <c r="F72" s="2">
         <v>1192.1795099999999</v>
       </c>
-      <c r="G72" s="3">
+      <c r="G72" s="2">
         <v>1319.21767</v>
       </c>
     </row>
@@ -2625,13 +2632,13 @@
       <c r="D73" s="2">
         <v>911.29</v>
       </c>
-      <c r="E73" s="3">
+      <c r="E73" s="2">
         <v>294.73352999999997</v>
       </c>
-      <c r="F73" s="3">
+      <c r="F73" s="2">
         <v>1409.52162</v>
       </c>
-      <c r="G73" s="3">
+      <c r="G73" s="2">
         <v>1514.96777</v>
       </c>
     </row>
@@ -2648,9 +2655,15 @@
       <c r="D74" s="2">
         <v>906</v>
       </c>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
+      <c r="E74" s="2">
+        <v>0</v>
+      </c>
+      <c r="F74" s="2">
+        <v>0</v>
+      </c>
+      <c r="G74" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
@@ -2665,13 +2678,13 @@
       <c r="D75" s="2">
         <v>887.65</v>
       </c>
-      <c r="E75" s="3">
+      <c r="E75" s="2">
         <v>105.24097</v>
       </c>
-      <c r="F75" s="3">
+      <c r="F75" s="2">
         <v>1039.095</v>
       </c>
-      <c r="G75" s="3">
+      <c r="G75" s="2">
         <v>1106.79458</v>
       </c>
     </row>
@@ -2688,13 +2701,13 @@
       <c r="D76" s="2">
         <v>911.08</v>
       </c>
-      <c r="E76" s="3">
+      <c r="E76" s="2">
         <v>97.204239999999999</v>
       </c>
-      <c r="F76" s="3">
+      <c r="F76" s="2">
         <v>978.73734999999999</v>
       </c>
-      <c r="G76" s="3">
+      <c r="G76" s="2">
         <v>1030.55297</v>
       </c>
     </row>
@@ -2711,13 +2724,13 @@
       <c r="D77" s="2">
         <v>901.33</v>
       </c>
-      <c r="E77" s="3">
+      <c r="E77" s="2">
         <v>90.438940000000002</v>
       </c>
-      <c r="F77" s="3">
+      <c r="F77" s="2">
         <v>955.98436000000004</v>
       </c>
-      <c r="G77" s="3">
+      <c r="G77" s="2">
         <v>993.92057</v>
       </c>
     </row>
@@ -2734,13 +2747,13 @@
       <c r="D78" s="2">
         <v>901.37</v>
       </c>
-      <c r="E78" s="3">
+      <c r="E78" s="2">
         <v>92.361220000000003</v>
       </c>
-      <c r="F78" s="3">
+      <c r="F78" s="2">
         <v>945.85311000000002</v>
       </c>
-      <c r="G78" s="3">
+      <c r="G78" s="2">
         <v>980.23811999999998</v>
       </c>
     </row>
@@ -2757,13 +2770,13 @@
       <c r="D79" s="2">
         <v>872.33</v>
       </c>
-      <c r="E79" s="3">
+      <c r="E79" s="2">
         <v>108.33758</v>
       </c>
-      <c r="F79" s="3">
+      <c r="F79" s="2">
         <v>1290.21558</v>
       </c>
-      <c r="G79" s="3">
+      <c r="G79" s="2">
         <v>1414.78655</v>
       </c>
     </row>
@@ -2780,13 +2793,13 @@
       <c r="D80" s="2">
         <v>865.96</v>
       </c>
-      <c r="E80" s="3">
+      <c r="E80" s="2">
         <v>90.573189999999997</v>
       </c>
-      <c r="F80" s="3">
+      <c r="F80" s="2">
         <v>1106.26243</v>
       </c>
-      <c r="G80" s="3">
+      <c r="G80" s="2">
         <v>1189.37345</v>
       </c>
     </row>
@@ -2803,13 +2816,13 @@
       <c r="D81" s="2">
         <v>870.98</v>
       </c>
-      <c r="E81" s="3">
+      <c r="E81" s="2">
         <v>114.67193</v>
       </c>
-      <c r="F81" s="3">
+      <c r="F81" s="2">
         <v>1253.49225</v>
       </c>
-      <c r="G81" s="3">
+      <c r="G81" s="2">
         <v>1396.2247400000001</v>
       </c>
     </row>
@@ -2826,13 +2839,13 @@
       <c r="D82" s="2">
         <v>870.57</v>
       </c>
-      <c r="E82" s="3">
+      <c r="E82" s="2">
         <v>71.363349999999997</v>
       </c>
-      <c r="F82" s="3">
+      <c r="F82" s="2">
         <v>946.23721</v>
       </c>
-      <c r="G82" s="3">
+      <c r="G82" s="2">
         <v>983.44866999999999</v>
       </c>
     </row>
@@ -2849,13 +2862,13 @@
       <c r="D83" s="2">
         <v>872.29</v>
       </c>
-      <c r="E83" s="3">
+      <c r="E83" s="2">
         <v>94.901309999999995</v>
       </c>
-      <c r="F83" s="3">
+      <c r="F83" s="2">
         <v>1133.9232300000001</v>
       </c>
-      <c r="G83" s="3">
+      <c r="G83" s="2">
         <v>1229.97387</v>
       </c>
     </row>
@@ -2872,13 +2885,13 @@
       <c r="D84" s="2">
         <v>869.95</v>
       </c>
-      <c r="E84" s="3">
+      <c r="E84" s="2">
         <v>79.649180000000001</v>
       </c>
-      <c r="F84" s="3">
+      <c r="F84" s="2">
         <v>1009.27651</v>
       </c>
-      <c r="G84" s="3">
+      <c r="G84" s="2">
         <v>1066.3247100000001</v>
       </c>
     </row>
@@ -2895,13 +2908,13 @@
       <c r="D85" s="2">
         <v>874.29</v>
       </c>
-      <c r="E85" s="3">
+      <c r="E85" s="2">
         <v>51.063270000000003</v>
       </c>
-      <c r="F85" s="3">
+      <c r="F85" s="2">
         <v>781.05587000000003</v>
       </c>
-      <c r="G85" s="3">
+      <c r="G85" s="2">
         <v>773.65565000000004</v>
       </c>
     </row>
@@ -2918,13 +2931,13 @@
       <c r="D86" s="2">
         <v>869.44</v>
       </c>
-      <c r="E86" s="3">
+      <c r="E86" s="2">
         <v>59.5518</v>
       </c>
-      <c r="F86" s="3">
+      <c r="F86" s="2">
         <v>855.34760000000006</v>
       </c>
-      <c r="G86" s="3">
+      <c r="G86" s="2">
         <v>866.81940999999995</v>
       </c>
     </row>
@@ -2941,13 +2954,13 @@
       <c r="D87" s="2">
         <v>866.9</v>
       </c>
-      <c r="E87" s="3">
+      <c r="E87" s="2">
         <v>113.67282</v>
       </c>
-      <c r="F87" s="3">
+      <c r="F87" s="2">
         <v>1190.6764900000001</v>
       </c>
-      <c r="G87" s="3">
+      <c r="G87" s="2">
         <v>1319.4387400000001</v>
       </c>
     </row>
@@ -2964,13 +2977,13 @@
       <c r="D88" s="2">
         <v>995</v>
       </c>
-      <c r="E88" s="3">
+      <c r="E88" s="2">
         <v>-3.7124999999999999</v>
       </c>
-      <c r="F88" s="3">
+      <c r="F88" s="2">
         <v>3531.8861000000002</v>
       </c>
-      <c r="G88" s="3">
+      <c r="G88" s="2">
         <v>4212.0260200000002</v>
       </c>
     </row>
@@ -2987,13 +3000,13 @@
       <c r="D89" s="2">
         <v>995</v>
       </c>
-      <c r="E89" s="3">
+      <c r="E89" s="2">
         <v>-3.7124999999999999</v>
       </c>
-      <c r="F89" s="3">
+      <c r="F89" s="2">
         <v>3531.8861000000002</v>
       </c>
-      <c r="G89" s="3">
+      <c r="G89" s="2">
         <v>4212.0260200000002</v>
       </c>
     </row>
@@ -3010,13 +3023,13 @@
       <c r="D90" s="2">
         <v>995</v>
       </c>
-      <c r="E90" s="3">
+      <c r="E90" s="2">
         <v>-3.7124999999999999</v>
       </c>
-      <c r="F90" s="3">
+      <c r="F90" s="2">
         <v>3531.8861000000002</v>
       </c>
-      <c r="G90" s="3">
+      <c r="G90" s="2">
         <v>4212.0260200000002</v>
       </c>
     </row>
@@ -3033,13 +3046,13 @@
       <c r="D91" s="2">
         <v>995</v>
       </c>
-      <c r="E91" s="3">
+      <c r="E91" s="2">
         <v>-3.7124999999999999</v>
       </c>
-      <c r="F91" s="3">
+      <c r="F91" s="2">
         <v>3531.8861000000002</v>
       </c>
-      <c r="G91" s="3">
+      <c r="G91" s="2">
         <v>4212.0260200000002</v>
       </c>
     </row>
@@ -3056,13 +3069,13 @@
       <c r="D92" s="2">
         <v>995</v>
       </c>
-      <c r="E92" s="3">
+      <c r="E92" s="2">
         <v>-3.7124999999999999</v>
       </c>
-      <c r="F92" s="3">
+      <c r="F92" s="2">
         <v>3531.8861000000002</v>
       </c>
-      <c r="G92" s="3">
+      <c r="G92" s="2">
         <v>4212.0260200000002</v>
       </c>
     </row>
@@ -3079,13 +3092,13 @@
       <c r="D93" s="2">
         <v>995</v>
       </c>
-      <c r="E93" s="3">
+      <c r="E93" s="2">
         <v>-3.7124999999999999</v>
       </c>
-      <c r="F93" s="3">
+      <c r="F93" s="2">
         <v>3531.8861000000002</v>
       </c>
-      <c r="G93" s="3">
+      <c r="G93" s="2">
         <v>4212.0260200000002</v>
       </c>
     </row>
@@ -3102,13 +3115,13 @@
       <c r="D94" s="2">
         <v>995</v>
       </c>
-      <c r="E94" s="3">
+      <c r="E94" s="2">
         <v>-3.7124999999999999</v>
       </c>
-      <c r="F94" s="3">
+      <c r="F94" s="2">
         <v>3531.8861000000002</v>
       </c>
-      <c r="G94" s="3">
+      <c r="G94" s="2">
         <v>4212.0260200000002</v>
       </c>
     </row>
@@ -3125,13 +3138,13 @@
       <c r="D95" s="2">
         <v>995</v>
       </c>
-      <c r="E95" s="3">
+      <c r="E95" s="2">
         <v>-3.7124999999999999</v>
       </c>
-      <c r="F95" s="3">
+      <c r="F95" s="2">
         <v>3531.8861000000002</v>
       </c>
-      <c r="G95" s="3">
+      <c r="G95" s="2">
         <v>4212.0260200000002</v>
       </c>
     </row>
@@ -3148,13 +3161,13 @@
       <c r="D96" s="2">
         <v>651.74</v>
       </c>
-      <c r="E96" s="3">
+      <c r="E96" s="2">
         <v>41.505130000000001</v>
       </c>
-      <c r="F96" s="3">
+      <c r="F96" s="2">
         <v>877.23563000000001</v>
       </c>
-      <c r="G96" s="3">
+      <c r="G96" s="2">
         <v>948.54510000000005</v>
       </c>
     </row>
@@ -3171,13 +3184,13 @@
       <c r="D97" s="2">
         <v>656.52</v>
       </c>
-      <c r="E97" s="3">
+      <c r="E97" s="2">
         <v>52.101509999999998</v>
       </c>
-      <c r="F97" s="3">
+      <c r="F97" s="2">
         <v>1028.4509599999999</v>
       </c>
-      <c r="G97" s="3">
+      <c r="G97" s="2">
         <v>1108.44949</v>
       </c>
     </row>
@@ -3194,13 +3207,13 @@
       <c r="D98" s="2">
         <v>900.53</v>
       </c>
-      <c r="E98" s="3">
+      <c r="E98" s="2">
         <v>147.82172</v>
       </c>
-      <c r="F98" s="3">
+      <c r="F98" s="2">
         <v>872.92118000000005</v>
       </c>
-      <c r="G98" s="3">
+      <c r="G98" s="2">
         <v>873.38602000000003</v>
       </c>
     </row>
@@ -3217,13 +3230,13 @@
       <c r="D99" s="2">
         <v>890.58</v>
       </c>
-      <c r="E99" s="3">
+      <c r="E99" s="2">
         <v>118.35751999999999</v>
       </c>
-      <c r="F99" s="3">
+      <c r="F99" s="2">
         <v>779.43859999999995</v>
       </c>
-      <c r="G99" s="3">
+      <c r="G99" s="2">
         <v>754.78877</v>
       </c>
     </row>
@@ -3240,13 +3253,13 @@
       <c r="D100" s="2">
         <v>885.46</v>
       </c>
-      <c r="E100" s="3">
+      <c r="E100" s="2">
         <v>97.330389999999994</v>
       </c>
-      <c r="F100" s="3">
+      <c r="F100" s="2">
         <v>689.04399999999998</v>
       </c>
-      <c r="G100" s="3">
+      <c r="G100" s="2">
         <v>641.54237000000001</v>
       </c>
     </row>
@@ -3263,13 +3276,13 @@
       <c r="D101" s="2">
         <v>322.33</v>
       </c>
-      <c r="E101" s="3">
+      <c r="E101" s="2">
         <v>69.377330000000001</v>
       </c>
-      <c r="F101" s="3">
+      <c r="F101" s="2">
         <v>1078.9416200000001</v>
       </c>
-      <c r="G101" s="3">
+      <c r="G101" s="2">
         <v>1193.5331100000001</v>
       </c>
     </row>
@@ -3286,13 +3299,13 @@
       <c r="D102" s="2">
         <v>220</v>
       </c>
-      <c r="E102" s="3">
+      <c r="E102" s="2">
         <v>69.508240000000001</v>
       </c>
-      <c r="F102" s="3">
+      <c r="F102" s="2">
         <v>1024.97696</v>
       </c>
-      <c r="G102" s="3">
+      <c r="G102" s="2">
         <v>1106.4743699999999</v>
       </c>
     </row>
@@ -3309,13 +3322,13 @@
       <c r="D103" s="2">
         <v>202.46</v>
       </c>
-      <c r="E103" s="3">
+      <c r="E103" s="2">
         <v>84.502009999999999</v>
       </c>
-      <c r="F103" s="3">
+      <c r="F103" s="2">
         <v>1096.7771399999999</v>
       </c>
-      <c r="G103" s="3">
+      <c r="G103" s="2">
         <v>1207.3726099999999</v>
       </c>
     </row>
@@ -3332,13 +3345,13 @@
       <c r="D104" s="2">
         <v>863</v>
       </c>
-      <c r="E104" s="3">
+      <c r="E104" s="2">
         <v>41.88796</v>
       </c>
-      <c r="F104" s="3">
+      <c r="F104" s="2">
         <v>640.69884999999999</v>
       </c>
-      <c r="G104" s="3">
+      <c r="G104" s="2">
         <v>602.48701000000005</v>
       </c>
     </row>
@@ -3355,13 +3368,13 @@
       <c r="D105" s="2">
         <v>840</v>
       </c>
-      <c r="E105" s="3">
+      <c r="E105" s="2">
         <v>24.30444</v>
       </c>
-      <c r="F105" s="3">
+      <c r="F105" s="2">
         <v>553.62972000000002</v>
       </c>
-      <c r="G105" s="3">
+      <c r="G105" s="2">
         <v>487.09294</v>
       </c>
     </row>
@@ -3378,13 +3391,13 @@
       <c r="D106" s="2">
         <v>227.33</v>
       </c>
-      <c r="E106" s="3">
+      <c r="E106" s="2">
         <v>29.077290000000001</v>
       </c>
-      <c r="F106" s="3">
+      <c r="F106" s="2">
         <v>663.34577999999999</v>
       </c>
-      <c r="G106" s="3">
+      <c r="G106" s="2">
         <v>640.21167000000003</v>
       </c>
     </row>
@@ -3401,13 +3414,13 @@
       <c r="D107" s="2">
         <v>180</v>
       </c>
-      <c r="E107" s="3">
+      <c r="E107" s="2">
         <v>78.419510000000002</v>
       </c>
-      <c r="F107" s="3">
+      <c r="F107" s="2">
         <v>822.15782000000002</v>
       </c>
-      <c r="G107" s="3">
+      <c r="G107" s="2">
         <v>822.48852999999997</v>
       </c>
     </row>
@@ -3424,13 +3437,13 @@
       <c r="D108" s="2">
         <v>709.83</v>
       </c>
-      <c r="E108" s="3">
+      <c r="E108" s="2">
         <v>31.104130000000001</v>
       </c>
-      <c r="F108" s="3">
+      <c r="F108" s="2">
         <v>522.51836000000003</v>
       </c>
-      <c r="G108" s="3">
+      <c r="G108" s="2">
         <v>456.98750000000001</v>
       </c>
     </row>
@@ -3447,13 +3460,13 @@
       <c r="D109" s="2">
         <v>324.67</v>
       </c>
-      <c r="E109" s="3">
+      <c r="E109" s="2">
         <v>38.40016</v>
       </c>
-      <c r="F109" s="3">
+      <c r="F109" s="2">
         <v>793.76701000000003</v>
       </c>
-      <c r="G109" s="3">
+      <c r="G109" s="2">
         <v>792.19101000000001</v>
       </c>
     </row>
@@ -3470,13 +3483,13 @@
       <c r="D110" s="2">
         <v>883.51</v>
       </c>
-      <c r="E110" s="3">
+      <c r="E110" s="2">
         <v>0.29937999999999998</v>
       </c>
-      <c r="F110" s="3">
+      <c r="F110" s="2">
         <v>520.59383000000003</v>
       </c>
-      <c r="G110" s="3">
+      <c r="G110" s="2">
         <v>449.67964000000001</v>
       </c>
     </row>
@@ -3493,13 +3506,13 @@
       <c r="D111" s="2">
         <v>888.79</v>
       </c>
-      <c r="E111" s="3">
+      <c r="E111" s="2">
         <v>80.246449999999996</v>
       </c>
-      <c r="F111" s="3">
+      <c r="F111" s="2">
         <v>886.42316000000005</v>
       </c>
-      <c r="G111" s="3">
+      <c r="G111" s="2">
         <v>913.66432999999995</v>
       </c>
     </row>
@@ -3516,13 +3529,13 @@
       <c r="D112" s="2">
         <v>165</v>
       </c>
-      <c r="E112" s="3">
+      <c r="E112" s="2">
         <v>97.501549999999995</v>
       </c>
-      <c r="F112" s="3">
+      <c r="F112" s="2">
         <v>1009.33542</v>
       </c>
-      <c r="G112" s="3">
+      <c r="G112" s="2">
         <v>1069.6439600000001</v>
       </c>
     </row>
@@ -3539,13 +3552,13 @@
       <c r="D113" s="2">
         <v>165</v>
       </c>
-      <c r="E113" s="3">
+      <c r="E113" s="2">
         <v>90.594830000000002</v>
       </c>
-      <c r="F113" s="3">
+      <c r="F113" s="2">
         <v>991.28566000000001</v>
       </c>
-      <c r="G113" s="3">
+      <c r="G113" s="2">
         <v>1047.25125</v>
       </c>
     </row>
@@ -3562,13 +3575,13 @@
       <c r="D114" s="2">
         <v>165</v>
       </c>
-      <c r="E114" s="3">
+      <c r="E114" s="2">
         <v>98.183639999999997</v>
       </c>
-      <c r="F114" s="3">
+      <c r="F114" s="2">
         <v>1015.74086</v>
       </c>
-      <c r="G114" s="3">
+      <c r="G114" s="2">
         <v>1078.1055799999999</v>
       </c>
     </row>
@@ -3585,13 +3598,13 @@
       <c r="D115" s="2">
         <v>165</v>
       </c>
-      <c r="E115" s="3">
+      <c r="E115" s="2">
         <v>91.865719999999996</v>
       </c>
-      <c r="F115" s="3">
+      <c r="F115" s="2">
         <v>975.32438000000002</v>
       </c>
-      <c r="G115" s="3">
+      <c r="G115" s="2">
         <v>1030.0664400000001</v>
       </c>
     </row>
@@ -3608,13 +3621,13 @@
       <c r="D116" s="2">
         <v>165</v>
       </c>
-      <c r="E116" s="3">
+      <c r="E116" s="2">
         <v>89.193200000000004</v>
       </c>
-      <c r="F116" s="3">
+      <c r="F116" s="2">
         <v>952.93786</v>
       </c>
-      <c r="G116" s="3">
+      <c r="G116" s="2">
         <v>1000.12405</v>
       </c>
     </row>
@@ -3631,13 +3644,13 @@
       <c r="D117" s="2">
         <v>165</v>
       </c>
-      <c r="E117" s="3">
+      <c r="E117" s="2">
         <v>95.571479999999994</v>
       </c>
-      <c r="F117" s="3">
+      <c r="F117" s="2">
         <v>987.57272999999998</v>
       </c>
-      <c r="G117" s="3">
+      <c r="G117" s="2">
         <v>1041.9241500000001</v>
       </c>
     </row>
@@ -3654,13 +3667,13 @@
       <c r="D118" s="2">
         <v>165</v>
       </c>
-      <c r="E118" s="3">
+      <c r="E118" s="2">
         <v>83.139060000000001</v>
       </c>
-      <c r="F118" s="3">
+      <c r="F118" s="2">
         <v>971.94101999999998</v>
       </c>
-      <c r="G118" s="3">
+      <c r="G118" s="2">
         <v>1030.2670000000001</v>
       </c>
     </row>
@@ -3677,13 +3690,13 @@
       <c r="D119" s="2">
         <v>165</v>
       </c>
-      <c r="E119" s="3">
+      <c r="E119" s="2">
         <v>86.960380000000001</v>
       </c>
-      <c r="F119" s="3">
+      <c r="F119" s="2">
         <v>949.41907000000003</v>
       </c>
-      <c r="G119" s="3">
+      <c r="G119" s="2">
         <v>997.13861999999995</v>
       </c>
     </row>
@@ -3700,13 +3713,13 @@
       <c r="D120" s="2">
         <v>165</v>
       </c>
-      <c r="E120" s="3">
+      <c r="E120" s="2">
         <v>92.871740000000003</v>
       </c>
-      <c r="F120" s="3">
+      <c r="F120" s="2">
         <v>985.42692999999997</v>
       </c>
-      <c r="G120" s="3">
+      <c r="G120" s="2">
         <v>1040.4312600000001</v>
       </c>
     </row>
@@ -3723,13 +3736,13 @@
       <c r="D121" s="2">
         <v>165</v>
       </c>
-      <c r="E121" s="3">
+      <c r="E121" s="2">
         <v>91.728039999999993</v>
       </c>
-      <c r="F121" s="3">
+      <c r="F121" s="2">
         <v>980.80745999999999</v>
       </c>
-      <c r="G121" s="3">
+      <c r="G121" s="2">
         <v>1035.51856</v>
       </c>
     </row>
@@ -3746,13 +3759,13 @@
       <c r="D122" s="2">
         <v>370</v>
       </c>
-      <c r="E122" s="3">
+      <c r="E122" s="2">
         <v>46.593539999999997</v>
       </c>
-      <c r="F122" s="3">
+      <c r="F122" s="2">
         <v>717.65364</v>
       </c>
-      <c r="G122" s="3">
+      <c r="G122" s="2">
         <v>697.20482000000004</v>
       </c>
     </row>
@@ -3769,13 +3782,13 @@
       <c r="D123" s="2">
         <v>456</v>
       </c>
-      <c r="E123" s="3">
+      <c r="E123" s="2">
         <v>55.974530000000001</v>
       </c>
-      <c r="F123" s="3">
+      <c r="F123" s="2">
         <v>803.01868999999999</v>
       </c>
-      <c r="G123" s="3">
+      <c r="G123" s="2">
         <v>806.94732999999997</v>
       </c>
     </row>
@@ -3792,13 +3805,13 @@
       <c r="D124" s="2">
         <v>845</v>
       </c>
-      <c r="E124" s="3">
+      <c r="E124" s="2">
         <v>36.930439999999997</v>
       </c>
-      <c r="F124" s="3">
+      <c r="F124" s="2">
         <v>698.16184999999996</v>
       </c>
-      <c r="G124" s="3">
+      <c r="G124" s="2">
         <v>669.85233000000005</v>
       </c>
     </row>
@@ -3815,13 +3828,13 @@
       <c r="D125" s="2">
         <v>845</v>
       </c>
-      <c r="E125" s="3">
+      <c r="E125" s="2">
         <v>55.620109999999997</v>
       </c>
-      <c r="F125" s="3">
+      <c r="F125" s="2">
         <v>756.23338000000001</v>
       </c>
-      <c r="G125" s="3">
+      <c r="G125" s="2">
         <v>745.82642999999996</v>
       </c>
     </row>
@@ -3838,13 +3851,13 @@
       <c r="D126" s="2">
         <v>845</v>
       </c>
-      <c r="E126" s="3">
+      <c r="E126" s="2">
         <v>73.029470000000003</v>
       </c>
-      <c r="F126" s="3">
+      <c r="F126" s="2">
         <v>834.62203</v>
       </c>
-      <c r="G126" s="3">
+      <c r="G126" s="2">
         <v>847.61706000000004</v>
       </c>
     </row>
@@ -3861,13 +3874,13 @@
       <c r="D127" s="2">
         <v>450</v>
       </c>
-      <c r="E127" s="3">
+      <c r="E127" s="2">
         <v>66.173749999999998</v>
       </c>
-      <c r="F127" s="3">
+      <c r="F127" s="2">
         <v>945.36153999999999</v>
       </c>
-      <c r="G127" s="3">
+      <c r="G127" s="2">
         <v>987.39417000000003</v>
       </c>
     </row>
@@ -3884,13 +3897,13 @@
       <c r="D128" s="2">
         <v>450</v>
       </c>
-      <c r="E128" s="3">
+      <c r="E128" s="2">
         <v>62.140500000000003</v>
       </c>
-      <c r="F128" s="3">
+      <c r="F128" s="2">
         <v>931.12222999999994</v>
       </c>
-      <c r="G128" s="3">
+      <c r="G128" s="2">
         <v>967.78536999999994</v>
       </c>
     </row>
@@ -3907,13 +3920,13 @@
       <c r="D129" s="2">
         <v>450</v>
       </c>
-      <c r="E129" s="3">
+      <c r="E129" s="2">
         <v>69.110259999999997</v>
       </c>
-      <c r="F129" s="3">
+      <c r="F129" s="2">
         <v>956.01424999999995</v>
       </c>
-      <c r="G129" s="3">
+      <c r="G129" s="2">
         <v>999.45385999999996</v>
       </c>
     </row>
@@ -3930,13 +3943,13 @@
       <c r="D130" s="2">
         <v>450</v>
       </c>
-      <c r="E130" s="3">
+      <c r="E130" s="2">
         <v>58.532800000000002</v>
       </c>
-      <c r="F130" s="3">
+      <c r="F130" s="2">
         <v>920.14088000000004</v>
       </c>
-      <c r="G130" s="3">
+      <c r="G130" s="2">
         <v>955.99950999999999</v>
       </c>
     </row>
@@ -3953,13 +3966,13 @@
       <c r="D131" s="2">
         <v>450</v>
       </c>
-      <c r="E131" s="3">
+      <c r="E131" s="2">
         <v>54.38843</v>
       </c>
-      <c r="F131" s="3">
+      <c r="F131" s="2">
         <v>901.95781999999997</v>
       </c>
-      <c r="G131" s="3">
+      <c r="G131" s="2">
         <v>931.05181000000005</v>
       </c>
     </row>
@@ -3976,13 +3989,13 @@
       <c r="D132" s="2">
         <v>450</v>
       </c>
-      <c r="E132" s="3">
+      <c r="E132" s="2">
         <v>61.56765</v>
       </c>
-      <c r="F132" s="3">
+      <c r="F132" s="2">
         <v>933.38172999999995</v>
       </c>
-      <c r="G132" s="3">
+      <c r="G132" s="2">
         <v>969.31545000000006</v>
       </c>
     </row>
@@ -3999,13 +4012,13 @@
       <c r="D133" s="2">
         <v>450</v>
       </c>
-      <c r="E133" s="3">
+      <c r="E133" s="2">
         <v>64.756900000000002</v>
       </c>
-      <c r="F133" s="3">
+      <c r="F133" s="2">
         <v>924.11273000000006</v>
       </c>
-      <c r="G133" s="3">
+      <c r="G133" s="2">
         <v>966.42352000000005</v>
       </c>
     </row>
@@ -4022,13 +4035,13 @@
       <c r="D134" s="2">
         <v>450</v>
       </c>
-      <c r="E134" s="3">
+      <c r="E134" s="2">
         <v>63.789879999999997</v>
       </c>
-      <c r="F134" s="3">
+      <c r="F134" s="2">
         <v>914.83558000000005</v>
       </c>
-      <c r="G134" s="3">
+      <c r="G134" s="2">
         <v>951.97581000000002</v>
       </c>
     </row>
@@ -4045,13 +4058,13 @@
       <c r="D135" s="2">
         <v>450</v>
       </c>
-      <c r="E135" s="3">
+      <c r="E135" s="2">
         <v>68.381600000000006</v>
       </c>
-      <c r="F135" s="3">
+      <c r="F135" s="2">
         <v>943.88905999999997</v>
       </c>
-      <c r="G135" s="3">
+      <c r="G135" s="2">
         <v>987.58330999999998</v>
       </c>
     </row>
@@ -4068,13 +4081,13 @@
       <c r="D136" s="2">
         <v>450</v>
       </c>
-      <c r="E136" s="3">
+      <c r="E136" s="2">
         <v>63.417639999999999</v>
       </c>
-      <c r="F136" s="3">
+      <c r="F136" s="2">
         <v>929.11897999999997</v>
       </c>
-      <c r="G136" s="3">
+      <c r="G136" s="2">
         <v>967.71463000000006</v>
       </c>
     </row>
@@ -4091,13 +4104,13 @@
       <c r="D137" s="2">
         <v>840</v>
       </c>
-      <c r="E137" s="3">
+      <c r="E137" s="2">
         <v>-0.82150000000000001</v>
       </c>
-      <c r="F137" s="3">
+      <c r="F137" s="2">
         <v>531.07858999999996</v>
       </c>
-      <c r="G137" s="3">
+      <c r="G137" s="2">
         <v>462.90652999999998</v>
       </c>
     </row>
@@ -4114,13 +4127,13 @@
       <c r="D138" s="2">
         <v>830</v>
       </c>
-      <c r="E138" s="3">
+      <c r="E138" s="2">
         <v>71.182540000000003</v>
       </c>
-      <c r="F138" s="3">
+      <c r="F138" s="2">
         <v>649.30093999999997</v>
       </c>
-      <c r="G138" s="3">
+      <c r="G138" s="2">
         <v>602.11006999999995</v>
       </c>
     </row>
@@ -4137,13 +4150,13 @@
       <c r="D139" s="2">
         <v>364.08</v>
       </c>
-      <c r="E139" s="3">
+      <c r="E139" s="2">
         <v>38.198630000000001</v>
       </c>
-      <c r="F139" s="3">
+      <c r="F139" s="2">
         <v>671.97681999999998</v>
       </c>
-      <c r="G139" s="3">
+      <c r="G139" s="2">
         <v>642.83272999999997</v>
       </c>
     </row>
@@ -4160,13 +4173,13 @@
       <c r="D140" s="2">
         <v>898.54</v>
       </c>
-      <c r="E140" s="3">
+      <c r="E140" s="2">
         <v>80.59187</v>
       </c>
-      <c r="F140" s="3">
+      <c r="F140" s="2">
         <v>784.49432999999999</v>
       </c>
-      <c r="G140" s="3">
+      <c r="G140" s="2">
         <v>779.01937999999996</v>
       </c>
     </row>
@@ -4183,13 +4196,13 @@
       <c r="D141" s="2">
         <v>830</v>
       </c>
-      <c r="E141" s="3">
+      <c r="E141" s="2">
         <v>24.505520000000001</v>
       </c>
-      <c r="F141" s="3">
+      <c r="F141" s="2">
         <v>445.31778000000003</v>
       </c>
-      <c r="G141" s="3">
+      <c r="G141" s="2">
         <v>356.71605</v>
       </c>
     </row>
@@ -4206,13 +4219,13 @@
       <c r="D142" s="2">
         <v>130</v>
       </c>
-      <c r="E142" s="3">
+      <c r="E142" s="2">
         <v>95.399959999999993</v>
       </c>
-      <c r="F142" s="3">
+      <c r="F142" s="2">
         <v>822.21927000000005</v>
       </c>
-      <c r="G142" s="3">
+      <c r="G142" s="2">
         <v>826.97820999999999</v>
       </c>
     </row>
@@ -4229,13 +4242,13 @@
       <c r="D143" s="2">
         <v>872.24</v>
       </c>
-      <c r="E143" s="3">
+      <c r="E143" s="2">
         <v>74.514300000000006</v>
       </c>
-      <c r="F143" s="3">
+      <c r="F143" s="2">
         <v>663.13103000000001</v>
       </c>
-      <c r="G143" s="3">
+      <c r="G143" s="2">
         <v>624.61014</v>
       </c>
     </row>
@@ -4252,13 +4265,13 @@
       <c r="D144" s="2">
         <v>403.1</v>
       </c>
-      <c r="E144" s="3">
+      <c r="E144" s="2">
         <v>37.935870000000001</v>
       </c>
-      <c r="F144" s="3">
+      <c r="F144" s="2">
         <v>677.81901000000005</v>
       </c>
-      <c r="G144" s="3">
+      <c r="G144" s="2">
         <v>650.34451999999999</v>
       </c>
     </row>
@@ -4275,13 +4288,13 @@
       <c r="D145" s="2">
         <v>902.56</v>
       </c>
-      <c r="E145" s="3">
+      <c r="E145" s="2">
         <v>73.277169999999998</v>
       </c>
-      <c r="F145" s="3">
+      <c r="F145" s="2">
         <v>670.87559999999996</v>
       </c>
-      <c r="G145" s="3">
+      <c r="G145" s="2">
         <v>637.03657999999996</v>
       </c>
     </row>
@@ -4298,13 +4311,13 @@
       <c r="D146" s="2">
         <v>201</v>
       </c>
-      <c r="E146" s="3">
+      <c r="E146" s="2">
         <v>41.472200000000001</v>
       </c>
-      <c r="F146" s="3">
+      <c r="F146" s="2">
         <v>827.30825000000004</v>
       </c>
-      <c r="G146" s="3">
+      <c r="G146" s="2">
         <v>833.82885999999996</v>
       </c>
     </row>
@@ -4321,13 +4334,13 @@
       <c r="D147" s="2">
         <v>849</v>
       </c>
-      <c r="E147" s="3">
+      <c r="E147" s="2">
         <v>-13.898250000000001</v>
       </c>
-      <c r="F147" s="3">
+      <c r="F147" s="2">
         <v>327.42838</v>
       </c>
-      <c r="G147" s="3">
+      <c r="G147" s="2">
         <v>232.10374999999999</v>
       </c>
     </row>
@@ -4344,13 +4357,13 @@
       <c r="D148" s="2">
         <v>840</v>
       </c>
-      <c r="E148" s="3">
+      <c r="E148" s="2">
         <v>-7.8560800000000004</v>
       </c>
-      <c r="F148" s="3">
+      <c r="F148" s="2">
         <v>481.86457000000001</v>
       </c>
-      <c r="G148" s="3">
+      <c r="G148" s="2">
         <v>404.23880000000003</v>
       </c>
     </row>
@@ -4367,13 +4380,13 @@
       <c r="D149" s="2">
         <v>250</v>
       </c>
-      <c r="E149" s="3">
+      <c r="E149" s="2">
         <v>46.257330000000003</v>
       </c>
-      <c r="F149" s="3">
+      <c r="F149" s="2">
         <v>945.21835999999996</v>
       </c>
-      <c r="G149" s="3">
+      <c r="G149" s="2">
         <v>989.66785000000004</v>
       </c>
     </row>
@@ -4390,13 +4403,13 @@
       <c r="D150" s="2">
         <v>160</v>
       </c>
-      <c r="E150" s="3">
+      <c r="E150" s="2">
         <v>60.384349999999998</v>
       </c>
-      <c r="F150" s="3">
+      <c r="F150" s="2">
         <v>912.69644000000005</v>
       </c>
-      <c r="G150" s="3">
+      <c r="G150" s="2">
         <v>945.67197999999996</v>
       </c>
     </row>
@@ -4413,9 +4426,15 @@
       <c r="D151" s="2">
         <v>320</v>
       </c>
-      <c r="E151" s="3"/>
-      <c r="F151" s="3"/>
-      <c r="G151" s="3"/>
+      <c r="E151" s="2">
+        <v>0</v>
+      </c>
+      <c r="F151" s="2">
+        <v>0</v>
+      </c>
+      <c r="G151" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
@@ -4430,13 +4449,13 @@
       <c r="D152" s="2">
         <v>435</v>
       </c>
-      <c r="E152" s="3">
+      <c r="E152" s="2">
         <v>56.53192</v>
       </c>
-      <c r="F152" s="3">
+      <c r="F152" s="2">
         <v>976.37275</v>
       </c>
-      <c r="G152" s="3">
+      <c r="G152" s="2">
         <v>1019.13749</v>
       </c>
     </row>
@@ -4453,13 +4472,13 @@
       <c r="D153" s="2">
         <v>324</v>
       </c>
-      <c r="E153" s="3">
+      <c r="E153" s="2">
         <v>51.145069999999997</v>
       </c>
-      <c r="F153" s="3">
+      <c r="F153" s="2">
         <v>940.3374</v>
       </c>
-      <c r="G153" s="3">
+      <c r="G153" s="2">
         <v>972.87469999999996</v>
       </c>
     </row>
@@ -4476,13 +4495,13 @@
       <c r="D154" s="2">
         <v>361</v>
       </c>
-      <c r="E154" s="3">
+      <c r="E154" s="2">
         <v>53.232939999999999</v>
       </c>
-      <c r="F154" s="3">
+      <c r="F154" s="2">
         <v>955.65659000000005</v>
       </c>
-      <c r="G154" s="3">
+      <c r="G154" s="2">
         <v>992.71022000000005</v>
       </c>
     </row>
@@ -4499,13 +4518,13 @@
       <c r="D155" s="2">
         <v>398</v>
       </c>
-      <c r="E155" s="3">
+      <c r="E155" s="2">
         <v>54.514499999999998</v>
       </c>
-      <c r="F155" s="3">
+      <c r="F155" s="2">
         <v>966.62543000000005</v>
       </c>
-      <c r="G155" s="3">
+      <c r="G155" s="2">
         <v>1006.58323</v>
       </c>
     </row>
@@ -4522,13 +4541,13 @@
       <c r="D156" s="2">
         <v>260</v>
       </c>
-      <c r="E156" s="3">
+      <c r="E156" s="2">
         <v>77.31532</v>
       </c>
-      <c r="F156" s="3">
+      <c r="F156" s="2">
         <v>931.48364000000004</v>
       </c>
-      <c r="G156" s="3">
+      <c r="G156" s="2">
         <v>1033.22102</v>
       </c>
     </row>
@@ -4545,13 +4564,13 @@
       <c r="D157" s="2">
         <v>877.82</v>
       </c>
-      <c r="E157" s="3">
+      <c r="E157" s="2">
         <v>-4.8858800000000002</v>
       </c>
-      <c r="F157" s="3">
+      <c r="F157" s="2">
         <v>425.12484000000001</v>
       </c>
-      <c r="G157" s="3">
+      <c r="G157" s="2">
         <v>342.87884000000003</v>
       </c>
     </row>
@@ -4568,13 +4587,13 @@
       <c r="D158" s="2">
         <v>325.83999999999997</v>
       </c>
-      <c r="E158" s="3">
+      <c r="E158" s="2">
         <v>46.67989</v>
       </c>
-      <c r="F158" s="3">
+      <c r="F158" s="2">
         <v>709.43140000000005</v>
       </c>
-      <c r="G158" s="3">
+      <c r="G158" s="2">
         <v>680.86659999999995</v>
       </c>
     </row>
@@ -4591,13 +4610,13 @@
       <c r="D159" s="2">
         <v>139.28</v>
       </c>
-      <c r="E159" s="3">
+      <c r="E159" s="2">
         <v>100.95616</v>
       </c>
-      <c r="F159" s="3">
+      <c r="F159" s="2">
         <v>1056.0173600000001</v>
       </c>
-      <c r="G159" s="3">
+      <c r="G159" s="2">
         <v>1168.53693</v>
       </c>
     </row>
@@ -4614,13 +4633,13 @@
       <c r="D160" s="2">
         <v>149</v>
       </c>
-      <c r="E160" s="3">
+      <c r="E160" s="2">
         <v>76.252560000000003</v>
       </c>
-      <c r="F160" s="3">
+      <c r="F160" s="2">
         <v>1025.9431099999999</v>
       </c>
-      <c r="G160" s="3">
+      <c r="G160" s="2">
         <v>1121.6369199999999</v>
       </c>
     </row>
@@ -4637,13 +4656,13 @@
       <c r="D161" s="2">
         <v>200</v>
       </c>
-      <c r="E161" s="3">
+      <c r="E161" s="2">
         <v>82.404269999999997</v>
       </c>
-      <c r="F161" s="3">
+      <c r="F161" s="2">
         <v>1109.71505</v>
       </c>
-      <c r="G161" s="3">
+      <c r="G161" s="2">
         <v>1239.2553700000001</v>
       </c>
     </row>
@@ -4660,13 +4679,13 @@
       <c r="D162" s="2">
         <v>112.25</v>
       </c>
-      <c r="E162" s="3">
+      <c r="E162" s="2">
         <v>93.868009999999998</v>
       </c>
-      <c r="F162" s="3">
+      <c r="F162" s="2">
         <v>1071.49451</v>
       </c>
-      <c r="G162" s="3">
+      <c r="G162" s="2">
         <v>1181.5035</v>
       </c>
     </row>
@@ -4683,13 +4702,13 @@
       <c r="D163" s="2">
         <v>183.52</v>
       </c>
-      <c r="E163" s="3">
+      <c r="E163" s="2">
         <v>36.497619999999998</v>
       </c>
-      <c r="F163" s="3">
+      <c r="F163" s="2">
         <v>803.10267999999996</v>
       </c>
-      <c r="G163" s="3">
+      <c r="G163" s="2">
         <v>804.52413999999999</v>
       </c>
     </row>
@@ -4706,13 +4725,13 @@
       <c r="D164" s="2">
         <v>161.41</v>
       </c>
-      <c r="E164" s="3">
+      <c r="E164" s="2">
         <v>90.522919999999999</v>
       </c>
-      <c r="F164" s="3">
+      <c r="F164" s="2">
         <v>1030.8917200000001</v>
       </c>
-      <c r="G164" s="3">
+      <c r="G164" s="2">
         <v>1108.0258799999999</v>
       </c>
     </row>
@@ -4729,13 +4748,13 @@
       <c r="D165" s="2">
         <v>212</v>
       </c>
-      <c r="E165" s="3">
+      <c r="E165" s="2">
         <v>83.934359999999998</v>
       </c>
-      <c r="F165" s="3">
+      <c r="F165" s="2">
         <v>1128.33917</v>
       </c>
-      <c r="G165" s="3">
+      <c r="G165" s="2">
         <v>1247.0399</v>
       </c>
     </row>
@@ -4752,13 +4771,13 @@
       <c r="D166" s="2">
         <v>118.5</v>
       </c>
-      <c r="E166" s="3">
+      <c r="E166" s="2">
         <v>114.98211999999999</v>
       </c>
-      <c r="F166" s="3">
+      <c r="F166" s="2">
         <v>1082.2521999999999</v>
       </c>
-      <c r="G166" s="3">
+      <c r="G166" s="2">
         <v>1183.81287</v>
       </c>
     </row>
@@ -4775,13 +4794,13 @@
       <c r="D167" s="2">
         <v>156.69999999999999</v>
       </c>
-      <c r="E167" s="3">
+      <c r="E167" s="2">
         <v>124.76308</v>
       </c>
-      <c r="F167" s="3">
+      <c r="F167" s="2">
         <v>1113.4349999999999</v>
       </c>
-      <c r="G167" s="3">
+      <c r="G167" s="2">
         <v>1228.17552</v>
       </c>
     </row>
@@ -4798,13 +4817,13 @@
       <c r="D168" s="2">
         <v>138.30000000000001</v>
       </c>
-      <c r="E168" s="3">
+      <c r="E168" s="2">
         <v>119.56726999999999</v>
       </c>
-      <c r="F168" s="3">
+      <c r="F168" s="2">
         <v>1096.7928400000001</v>
       </c>
-      <c r="G168" s="3">
+      <c r="G168" s="2">
         <v>1203.7130299999999</v>
       </c>
     </row>
@@ -4821,13 +4840,13 @@
       <c r="D169" s="2">
         <v>145</v>
       </c>
-      <c r="E169" s="3">
+      <c r="E169" s="2">
         <v>122.19844999999999</v>
       </c>
-      <c r="F169" s="3">
+      <c r="F169" s="2">
         <v>1108.9523099999999</v>
       </c>
-      <c r="G169" s="3">
+      <c r="G169" s="2">
         <v>1221.19759</v>
       </c>
     </row>
@@ -4844,13 +4863,13 @@
       <c r="D170" s="2">
         <v>258.11</v>
       </c>
-      <c r="E170" s="3">
+      <c r="E170" s="2">
         <v>146.54954000000001</v>
       </c>
-      <c r="F170" s="3">
+      <c r="F170" s="2">
         <v>946.67961000000003</v>
       </c>
-      <c r="G170" s="3">
+      <c r="G170" s="2">
         <v>952.40196000000003</v>
       </c>
     </row>
@@ -4867,13 +4886,13 @@
       <c r="D171" s="2">
         <v>222</v>
       </c>
-      <c r="E171" s="3">
+      <c r="E171" s="2">
         <v>137.33089000000001</v>
       </c>
-      <c r="F171" s="3">
+      <c r="F171" s="2">
         <v>944.80776000000003</v>
       </c>
-      <c r="G171" s="3">
+      <c r="G171" s="2">
         <v>951.34226000000001</v>
       </c>
     </row>
@@ -4890,13 +4909,13 @@
       <c r="D172" s="2">
         <v>265</v>
       </c>
-      <c r="E172" s="3">
+      <c r="E172" s="2">
         <v>140.16818000000001</v>
       </c>
-      <c r="F172" s="3">
+      <c r="F172" s="2">
         <v>941.21596</v>
       </c>
-      <c r="G172" s="3">
+      <c r="G172" s="2">
         <v>946.75824</v>
       </c>
     </row>
@@ -4913,13 +4932,13 @@
       <c r="D173" s="2">
         <v>248</v>
       </c>
-      <c r="E173" s="3">
+      <c r="E173" s="2">
         <v>94.743579999999994</v>
       </c>
-      <c r="F173" s="3">
+      <c r="F173" s="2">
         <v>1067.0728200000001</v>
       </c>
-      <c r="G173" s="3">
+      <c r="G173" s="2">
         <v>1164.5875599999999</v>
       </c>
     </row>
@@ -4936,13 +4955,13 @@
       <c r="D174" s="2">
         <v>232.07</v>
       </c>
-      <c r="E174" s="3">
+      <c r="E174" s="2">
         <v>83.050730000000001</v>
       </c>
-      <c r="F174" s="3">
+      <c r="F174" s="2">
         <v>984.83271999999999</v>
       </c>
-      <c r="G174" s="3">
+      <c r="G174" s="2">
         <v>1055.1437100000001</v>
       </c>
     </row>
@@ -4959,13 +4978,13 @@
       <c r="D175" s="2">
         <v>632</v>
       </c>
-      <c r="E175" s="3">
+      <c r="E175" s="2">
         <v>77.503979999999999</v>
       </c>
-      <c r="F175" s="3">
+      <c r="F175" s="2">
         <v>1175.5896299999999</v>
       </c>
-      <c r="G175" s="3">
+      <c r="G175" s="2">
         <v>1291.5400500000001</v>
       </c>
     </row>
@@ -4982,13 +5001,13 @@
       <c r="D176" s="2">
         <v>525</v>
       </c>
-      <c r="E176" s="3">
+      <c r="E176" s="2">
         <v>75.43262</v>
       </c>
-      <c r="F176" s="3">
+      <c r="F176" s="2">
         <v>1145.64688</v>
       </c>
-      <c r="G176" s="3">
+      <c r="G176" s="2">
         <v>1249.98378</v>
       </c>
     </row>
@@ -5005,13 +5024,13 @@
       <c r="D177" s="2">
         <v>662</v>
       </c>
-      <c r="E177" s="3">
+      <c r="E177" s="2">
         <v>82.458960000000005</v>
       </c>
-      <c r="F177" s="3">
+      <c r="F177" s="2">
         <v>1207.6604299999999</v>
       </c>
-      <c r="G177" s="3">
+      <c r="G177" s="2">
         <v>1333.7865099999999</v>
       </c>
     </row>
@@ -5028,9 +5047,15 @@
       <c r="D178" s="2">
         <v>418</v>
       </c>
-      <c r="E178" s="3"/>
-      <c r="F178" s="3"/>
-      <c r="G178" s="3"/>
+      <c r="E178" s="2">
+        <v>0</v>
+      </c>
+      <c r="F178" s="2">
+        <v>0</v>
+      </c>
+      <c r="G178" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
@@ -5045,13 +5070,13 @@
       <c r="D179" s="2">
         <v>414</v>
       </c>
-      <c r="E179" s="3">
+      <c r="E179" s="2">
         <v>89.739720000000005</v>
       </c>
-      <c r="F179" s="3">
+      <c r="F179" s="2">
         <v>1064.1295299999999</v>
       </c>
-      <c r="G179" s="3">
+      <c r="G179" s="2">
         <v>1136.9253699999999</v>
       </c>
     </row>
@@ -5068,13 +5093,13 @@
       <c r="D180" s="2">
         <v>418</v>
       </c>
-      <c r="E180" s="3">
+      <c r="E180" s="2">
         <v>107.29031000000001</v>
       </c>
-      <c r="F180" s="3">
+      <c r="F180" s="2">
         <v>1099.4960900000001</v>
       </c>
-      <c r="G180" s="3">
+      <c r="G180" s="2">
         <v>1185.8258599999999</v>
       </c>
     </row>
@@ -5091,9 +5116,15 @@
       <c r="D181" s="2">
         <v>260.38</v>
       </c>
-      <c r="E181" s="3"/>
-      <c r="F181" s="3"/>
-      <c r="G181" s="3"/>
+      <c r="E181" s="2">
+        <v>0</v>
+      </c>
+      <c r="F181" s="2">
+        <v>0</v>
+      </c>
+      <c r="G181" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
@@ -5108,13 +5139,13 @@
       <c r="D182" s="2">
         <v>259</v>
       </c>
-      <c r="E182" s="3">
+      <c r="E182" s="2">
         <v>126.16269</v>
       </c>
-      <c r="F182" s="3">
+      <c r="F182" s="2">
         <v>1196.2801300000001</v>
       </c>
-      <c r="G182" s="3">
+      <c r="G182" s="2">
         <v>1308.4807000000001</v>
       </c>
     </row>
@@ -5131,13 +5162,13 @@
       <c r="D183" s="2">
         <v>261</v>
       </c>
-      <c r="E183" s="3">
+      <c r="E183" s="2">
         <v>167.53682000000001</v>
       </c>
-      <c r="F183" s="3">
+      <c r="F183" s="2">
         <v>1188.50422</v>
       </c>
-      <c r="G183" s="3">
+      <c r="G183" s="2">
         <v>1291.3612499999999</v>
       </c>
     </row>
@@ -5154,13 +5185,13 @@
       <c r="D184" s="2">
         <v>256</v>
       </c>
-      <c r="E184" s="3">
+      <c r="E184" s="2">
         <v>137.65004999999999</v>
       </c>
-      <c r="F184" s="3">
+      <c r="F184" s="2">
         <v>1203.25578</v>
       </c>
-      <c r="G184" s="3">
+      <c r="G184" s="2">
         <v>1313.71325</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix :  - Excel : Deleted Five lines because of null columns
</commit_message>
<xml_diff>
--- a/CVB-Tabel.xlsx
+++ b/CVB-Tabel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghanm\Documents\ILVO Projects\Drupal RekeningTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B046EE03-506B-4B97-B61E-2A295D7901CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B4AD13-76C2-4563-A882-3406ABAB992C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="189">
   <si>
     <t>Naam</t>
   </si>
@@ -209,9 +209,6 @@
     <t>Palmpitschilfers, RC &gt; 180 g/kg</t>
   </si>
   <si>
-    <t>Palmpitschroot</t>
-  </si>
-  <si>
     <t xml:space="preserve">Palmpitschroot, RC &lt; 190 g/kg   </t>
   </si>
   <si>
@@ -266,9 +263,6 @@
     <t>Tarweglutenmeel</t>
   </si>
   <si>
-    <t>Tarweglutenvoer, gedroogd</t>
-  </si>
-  <si>
     <t>Tarweglutenvoer, gedroogd, RAS &lt; 40 g/kg</t>
   </si>
   <si>
@@ -494,9 +488,6 @@
     <t>Snijgraan, vers</t>
   </si>
   <si>
-    <t>Snijmais, kuil</t>
-  </si>
-  <si>
     <t>Snijmais, kuil, DS &gt; 420 g/kg</t>
   </si>
   <si>
@@ -578,16 +569,10 @@
     <t>Corn Cob Mix (CCM), kuil, zonder spil, RC &lt; 40 g/kg DS</t>
   </si>
   <si>
-    <t>Maisglutenvoer, vers en kuil</t>
-  </si>
-  <si>
     <t xml:space="preserve">Maisglutenvoer, vers en kuil, ZETew &lt; 200 g/kg DS   </t>
   </si>
   <si>
     <t xml:space="preserve">Maisglutenvoer, vers en kuil, ZETew &gt; 200 g/kg DS   </t>
-  </si>
-  <si>
-    <t>Tarwegistconcentraat</t>
   </si>
   <si>
     <t>Tarwegistconcentraat, RE &lt; 275 g/kg DS</t>
@@ -949,10 +934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G184"/>
+  <dimension ref="A1:G179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2101,16 +2086,16 @@
         <v>9</v>
       </c>
       <c r="D50" s="2">
-        <v>879.56</v>
+        <v>892.77</v>
       </c>
       <c r="E50" s="2">
-        <v>0</v>
+        <v>134.25316000000001</v>
       </c>
       <c r="F50" s="2">
-        <v>0</v>
+        <v>975.24495000000002</v>
       </c>
       <c r="G50" s="2">
-        <v>0</v>
+        <v>1017.70763</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2124,21 +2109,21 @@
         <v>9</v>
       </c>
       <c r="D51" s="2">
-        <v>892.77</v>
+        <v>875.52</v>
       </c>
       <c r="E51" s="2">
-        <v>134.25316000000001</v>
+        <v>125.20237</v>
       </c>
       <c r="F51" s="2">
-        <v>975.24495000000002</v>
+        <v>869.51274000000001</v>
       </c>
       <c r="G51" s="2">
-        <v>1017.70763</v>
+        <v>880.97877000000005</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>182</v>
       </c>
       <c r="B52" t="s">
         <v>8</v>
@@ -2147,21 +2132,21 @@
         <v>9</v>
       </c>
       <c r="D52" s="2">
-        <v>875.52</v>
+        <v>924.67</v>
       </c>
       <c r="E52" s="2">
-        <v>125.20237</v>
+        <v>37.284390000000002</v>
       </c>
       <c r="F52" s="2">
-        <v>869.51274000000001</v>
+        <v>2028.4947099999999</v>
       </c>
       <c r="G52" s="2">
-        <v>880.97877000000005</v>
+        <v>2304.1664000000001</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B53" t="s">
         <v>8</v>
@@ -2170,21 +2155,21 @@
         <v>9</v>
       </c>
       <c r="D53" s="2">
-        <v>924.67</v>
+        <v>902.31</v>
       </c>
       <c r="E53" s="2">
-        <v>37.284390000000002</v>
+        <v>131.13724999999999</v>
       </c>
       <c r="F53" s="2">
-        <v>2028.4947099999999</v>
+        <v>1169.60465</v>
       </c>
       <c r="G53" s="2">
-        <v>2304.1664000000001</v>
+        <v>1243.39733</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B54" t="s">
         <v>8</v>
@@ -2193,21 +2178,21 @@
         <v>9</v>
       </c>
       <c r="D54" s="2">
-        <v>902.31</v>
+        <v>877.02</v>
       </c>
       <c r="E54" s="2">
-        <v>131.13724999999999</v>
+        <v>295.27890000000002</v>
       </c>
       <c r="F54" s="2">
-        <v>1169.60465</v>
+        <v>944.27094999999997</v>
       </c>
       <c r="G54" s="2">
-        <v>1243.39733</v>
+        <v>966.06867</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
@@ -2216,21 +2201,21 @@
         <v>9</v>
       </c>
       <c r="D55" s="2">
-        <v>877.02</v>
+        <v>881.6</v>
       </c>
       <c r="E55" s="2">
-        <v>295.27890000000002</v>
+        <v>144.71459999999999</v>
       </c>
       <c r="F55" s="2">
-        <v>944.27094999999997</v>
+        <v>972.55381</v>
       </c>
       <c r="G55" s="2">
-        <v>966.06867</v>
+        <v>1004.14373</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B56" t="s">
         <v>8</v>
@@ -2239,21 +2224,21 @@
         <v>9</v>
       </c>
       <c r="D56" s="2">
-        <v>881.6</v>
+        <v>896.92</v>
       </c>
       <c r="E56" s="2">
-        <v>144.71459999999999</v>
+        <v>157.26173</v>
       </c>
       <c r="F56" s="2">
-        <v>972.55381</v>
+        <v>950.41858999999999</v>
       </c>
       <c r="G56" s="2">
-        <v>1004.14373</v>
+        <v>977.3827</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>191</v>
+        <v>59</v>
       </c>
       <c r="B57" t="s">
         <v>8</v>
@@ -2262,16 +2247,16 @@
         <v>9</v>
       </c>
       <c r="D57" s="2">
-        <v>896.92</v>
+        <v>869.5</v>
       </c>
       <c r="E57" s="2">
-        <v>157.26173</v>
+        <v>111.05419000000001</v>
       </c>
       <c r="F57" s="2">
-        <v>950.41858999999999</v>
+        <v>1158.24134</v>
       </c>
       <c r="G57" s="2">
-        <v>977.3827</v>
+        <v>1276.77638</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2285,16 +2270,16 @@
         <v>9</v>
       </c>
       <c r="D58" s="2">
-        <v>869.5</v>
+        <v>898.9</v>
       </c>
       <c r="E58" s="2">
-        <v>111.05419000000001</v>
+        <v>118.97512999999999</v>
       </c>
       <c r="F58" s="2">
-        <v>1158.24134</v>
+        <v>1585.3824400000001</v>
       </c>
       <c r="G58" s="2">
-        <v>1276.77638</v>
+        <v>1763.18237</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2311,13 +2296,13 @@
         <v>898.9</v>
       </c>
       <c r="E59" s="2">
-        <v>118.97512999999999</v>
+        <v>173.58584999999999</v>
       </c>
       <c r="F59" s="2">
-        <v>1585.3824400000001</v>
+        <v>1585.39041</v>
       </c>
       <c r="G59" s="2">
-        <v>1763.18237</v>
+        <v>1763.1896300000001</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2331,16 +2316,16 @@
         <v>9</v>
       </c>
       <c r="D60" s="2">
-        <v>898.9</v>
+        <v>883.03</v>
       </c>
       <c r="E60" s="2">
-        <v>173.58584999999999</v>
+        <v>89.994929999999997</v>
       </c>
       <c r="F60" s="2">
-        <v>1585.39041</v>
+        <v>1058.2932499999999</v>
       </c>
       <c r="G60" s="2">
-        <v>1763.1896300000001</v>
+        <v>1123.3379199999999</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2354,16 +2339,16 @@
         <v>9</v>
       </c>
       <c r="D61" s="2">
-        <v>883.03</v>
+        <v>886.79</v>
       </c>
       <c r="E61" s="2">
-        <v>89.994929999999997</v>
+        <v>80.40634</v>
       </c>
       <c r="F61" s="2">
-        <v>1058.2932499999999</v>
+        <v>1003.38276</v>
       </c>
       <c r="G61" s="2">
-        <v>1123.3379199999999</v>
+        <v>1053.6854800000001</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2377,16 +2362,16 @@
         <v>9</v>
       </c>
       <c r="D62" s="2">
-        <v>886.79</v>
+        <v>886.07</v>
       </c>
       <c r="E62" s="2">
-        <v>80.40634</v>
+        <v>81.533680000000004</v>
       </c>
       <c r="F62" s="2">
-        <v>1003.38276</v>
+        <v>1020.99271</v>
       </c>
       <c r="G62" s="2">
-        <v>1053.6854800000001</v>
+        <v>1076.0888199999999</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2400,16 +2385,16 @@
         <v>9</v>
       </c>
       <c r="D63" s="2">
-        <v>886.07</v>
+        <v>872</v>
       </c>
       <c r="E63" s="2">
-        <v>81.533680000000004</v>
+        <v>435.53834000000001</v>
       </c>
       <c r="F63" s="2">
-        <v>1020.99271</v>
+        <v>1136.45886</v>
       </c>
       <c r="G63" s="2">
-        <v>1076.0888199999999</v>
+        <v>1213.64491</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2423,16 +2408,16 @@
         <v>9</v>
       </c>
       <c r="D64" s="2">
-        <v>872</v>
+        <v>873.27</v>
       </c>
       <c r="E64" s="2">
-        <v>435.53834000000001</v>
+        <v>424.35309000000001</v>
       </c>
       <c r="F64" s="2">
-        <v>1136.45886</v>
+        <v>1139.27071</v>
       </c>
       <c r="G64" s="2">
-        <v>1213.64491</v>
+        <v>1215.7613899999999</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2446,16 +2431,16 @@
         <v>9</v>
       </c>
       <c r="D65" s="2">
-        <v>873.27</v>
+        <v>881.51</v>
       </c>
       <c r="E65" s="2">
-        <v>424.35309000000001</v>
+        <v>269.77168</v>
       </c>
       <c r="F65" s="2">
-        <v>1139.27071</v>
+        <v>1152.06258</v>
       </c>
       <c r="G65" s="2">
-        <v>1215.7613899999999</v>
+        <v>1235.71163</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2469,16 +2454,16 @@
         <v>9</v>
       </c>
       <c r="D66" s="2">
-        <v>881.51</v>
+        <v>878.07</v>
       </c>
       <c r="E66" s="2">
-        <v>269.77168</v>
+        <v>279.47091999999998</v>
       </c>
       <c r="F66" s="2">
-        <v>1152.06258</v>
+        <v>1153.73552</v>
       </c>
       <c r="G66" s="2">
-        <v>1235.71163</v>
+        <v>1235.4047499999999</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2492,16 +2477,16 @@
         <v>9</v>
       </c>
       <c r="D67" s="2">
-        <v>878.07</v>
+        <v>877.54</v>
       </c>
       <c r="E67" s="2">
-        <v>279.47091999999998</v>
+        <v>246.25176999999999</v>
       </c>
       <c r="F67" s="2">
-        <v>1153.73552</v>
+        <v>1138.65851</v>
       </c>
       <c r="G67" s="2">
-        <v>1235.4047499999999</v>
+        <v>1220.1039499999999</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2515,16 +2500,16 @@
         <v>9</v>
       </c>
       <c r="D68" s="2">
-        <v>877.54</v>
+        <v>879.76</v>
       </c>
       <c r="E68" s="2">
-        <v>246.25176999999999</v>
+        <v>253.47504000000001</v>
       </c>
       <c r="F68" s="2">
-        <v>1138.65851</v>
+        <v>1146.0111899999999</v>
       </c>
       <c r="G68" s="2">
-        <v>1220.1039499999999</v>
+        <v>1228.6584</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2538,16 +2523,16 @@
         <v>9</v>
       </c>
       <c r="D69" s="2">
-        <v>879.76</v>
+        <v>877.34</v>
       </c>
       <c r="E69" s="2">
-        <v>253.47504000000001</v>
+        <v>268.85194999999999</v>
       </c>
       <c r="F69" s="2">
-        <v>1146.0111899999999</v>
+        <v>1153.9401399999999</v>
       </c>
       <c r="G69" s="2">
-        <v>1228.6584</v>
+        <v>1236.3154</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2561,16 +2546,16 @@
         <v>9</v>
       </c>
       <c r="D70" s="2">
-        <v>877.34</v>
+        <v>871.58</v>
       </c>
       <c r="E70" s="2">
-        <v>268.85194999999999</v>
+        <v>103.04266</v>
       </c>
       <c r="F70" s="2">
-        <v>1153.9401399999999</v>
+        <v>1156.9828500000001</v>
       </c>
       <c r="G70" s="2">
-        <v>1236.3154</v>
+        <v>1270.1314199999999</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2584,16 +2569,16 @@
         <v>9</v>
       </c>
       <c r="D71" s="2">
-        <v>871.58</v>
+        <v>866.55</v>
       </c>
       <c r="E71" s="2">
-        <v>103.04266</v>
+        <v>114.29871</v>
       </c>
       <c r="F71" s="2">
-        <v>1156.9828500000001</v>
+        <v>1192.1795099999999</v>
       </c>
       <c r="G71" s="2">
-        <v>1270.1314199999999</v>
+        <v>1319.21767</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2607,16 +2592,16 @@
         <v>9</v>
       </c>
       <c r="D72" s="2">
-        <v>866.55</v>
+        <v>911.29</v>
       </c>
       <c r="E72" s="2">
-        <v>114.29871</v>
+        <v>294.73352999999997</v>
       </c>
       <c r="F72" s="2">
-        <v>1192.1795099999999</v>
+        <v>1409.52162</v>
       </c>
       <c r="G72" s="2">
-        <v>1319.21767</v>
+        <v>1514.96777</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2630,16 +2615,16 @@
         <v>9</v>
       </c>
       <c r="D73" s="2">
-        <v>911.29</v>
+        <v>887.65</v>
       </c>
       <c r="E73" s="2">
-        <v>294.73352999999997</v>
+        <v>105.24097</v>
       </c>
       <c r="F73" s="2">
-        <v>1409.52162</v>
+        <v>1039.095</v>
       </c>
       <c r="G73" s="2">
-        <v>1514.96777</v>
+        <v>1106.79458</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2653,16 +2638,16 @@
         <v>9</v>
       </c>
       <c r="D74" s="2">
-        <v>906</v>
+        <v>911.08</v>
       </c>
       <c r="E74" s="2">
-        <v>0</v>
+        <v>97.204239999999999</v>
       </c>
       <c r="F74" s="2">
-        <v>0</v>
+        <v>978.73734999999999</v>
       </c>
       <c r="G74" s="2">
-        <v>0</v>
+        <v>1030.55297</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2676,16 +2661,16 @@
         <v>9</v>
       </c>
       <c r="D75" s="2">
-        <v>887.65</v>
+        <v>901.33</v>
       </c>
       <c r="E75" s="2">
-        <v>105.24097</v>
+        <v>90.438940000000002</v>
       </c>
       <c r="F75" s="2">
-        <v>1039.095</v>
+        <v>955.98436000000004</v>
       </c>
       <c r="G75" s="2">
-        <v>1106.79458</v>
+        <v>993.92057</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2699,16 +2684,16 @@
         <v>9</v>
       </c>
       <c r="D76" s="2">
-        <v>911.08</v>
+        <v>901.37</v>
       </c>
       <c r="E76" s="2">
-        <v>97.204239999999999</v>
+        <v>92.361220000000003</v>
       </c>
       <c r="F76" s="2">
-        <v>978.73734999999999</v>
+        <v>945.85311000000002</v>
       </c>
       <c r="G76" s="2">
-        <v>1030.55297</v>
+        <v>980.23811999999998</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2722,16 +2707,16 @@
         <v>9</v>
       </c>
       <c r="D77" s="2">
-        <v>901.33</v>
+        <v>872.33</v>
       </c>
       <c r="E77" s="2">
-        <v>90.438940000000002</v>
+        <v>108.33758</v>
       </c>
       <c r="F77" s="2">
-        <v>955.98436000000004</v>
+        <v>1290.21558</v>
       </c>
       <c r="G77" s="2">
-        <v>993.92057</v>
+        <v>1414.78655</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2745,16 +2730,16 @@
         <v>9</v>
       </c>
       <c r="D78" s="2">
-        <v>901.37</v>
+        <v>865.96</v>
       </c>
       <c r="E78" s="2">
-        <v>92.361220000000003</v>
+        <v>90.573189999999997</v>
       </c>
       <c r="F78" s="2">
-        <v>945.85311000000002</v>
+        <v>1106.26243</v>
       </c>
       <c r="G78" s="2">
-        <v>980.23811999999998</v>
+        <v>1189.37345</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2768,16 +2753,16 @@
         <v>9</v>
       </c>
       <c r="D79" s="2">
-        <v>872.33</v>
+        <v>870.98</v>
       </c>
       <c r="E79" s="2">
-        <v>108.33758</v>
+        <v>114.67193</v>
       </c>
       <c r="F79" s="2">
-        <v>1290.21558</v>
+        <v>1253.49225</v>
       </c>
       <c r="G79" s="2">
-        <v>1414.78655</v>
+        <v>1396.2247400000001</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2791,16 +2776,16 @@
         <v>9</v>
       </c>
       <c r="D80" s="2">
-        <v>865.96</v>
+        <v>870.57</v>
       </c>
       <c r="E80" s="2">
-        <v>90.573189999999997</v>
+        <v>71.363349999999997</v>
       </c>
       <c r="F80" s="2">
-        <v>1106.26243</v>
+        <v>946.23721</v>
       </c>
       <c r="G80" s="2">
-        <v>1189.37345</v>
+        <v>983.44866999999999</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2814,16 +2799,16 @@
         <v>9</v>
       </c>
       <c r="D81" s="2">
-        <v>870.98</v>
+        <v>872.29</v>
       </c>
       <c r="E81" s="2">
-        <v>114.67193</v>
+        <v>94.901309999999995</v>
       </c>
       <c r="F81" s="2">
-        <v>1253.49225</v>
+        <v>1133.9232300000001</v>
       </c>
       <c r="G81" s="2">
-        <v>1396.2247400000001</v>
+        <v>1229.97387</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2837,16 +2822,16 @@
         <v>9</v>
       </c>
       <c r="D82" s="2">
-        <v>870.57</v>
+        <v>869.95</v>
       </c>
       <c r="E82" s="2">
-        <v>71.363349999999997</v>
+        <v>79.649180000000001</v>
       </c>
       <c r="F82" s="2">
-        <v>946.23721</v>
+        <v>1009.27651</v>
       </c>
       <c r="G82" s="2">
-        <v>983.44866999999999</v>
+        <v>1066.3247100000001</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2860,16 +2845,16 @@
         <v>9</v>
       </c>
       <c r="D83" s="2">
-        <v>872.29</v>
+        <v>874.29</v>
       </c>
       <c r="E83" s="2">
-        <v>94.901309999999995</v>
+        <v>51.063270000000003</v>
       </c>
       <c r="F83" s="2">
-        <v>1133.9232300000001</v>
+        <v>781.05587000000003</v>
       </c>
       <c r="G83" s="2">
-        <v>1229.97387</v>
+        <v>773.65565000000004</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2883,16 +2868,16 @@
         <v>9</v>
       </c>
       <c r="D84" s="2">
-        <v>869.95</v>
+        <v>869.44</v>
       </c>
       <c r="E84" s="2">
-        <v>79.649180000000001</v>
+        <v>59.5518</v>
       </c>
       <c r="F84" s="2">
-        <v>1009.27651</v>
+        <v>855.34760000000006</v>
       </c>
       <c r="G84" s="2">
-        <v>1066.3247100000001</v>
+        <v>866.81940999999995</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2906,16 +2891,16 @@
         <v>9</v>
       </c>
       <c r="D85" s="2">
-        <v>874.29</v>
+        <v>866.9</v>
       </c>
       <c r="E85" s="2">
-        <v>51.063270000000003</v>
+        <v>113.67282</v>
       </c>
       <c r="F85" s="2">
-        <v>781.05587000000003</v>
+        <v>1190.6764900000001</v>
       </c>
       <c r="G85" s="2">
-        <v>773.65565000000004</v>
+        <v>1319.4387400000001</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -2929,16 +2914,16 @@
         <v>9</v>
       </c>
       <c r="D86" s="2">
-        <v>869.44</v>
+        <v>995</v>
       </c>
       <c r="E86" s="2">
-        <v>59.5518</v>
+        <v>-3.7124999999999999</v>
       </c>
       <c r="F86" s="2">
-        <v>855.34760000000006</v>
+        <v>3531.8861000000002</v>
       </c>
       <c r="G86" s="2">
-        <v>866.81940999999995</v>
+        <v>4212.0260200000002</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -2952,16 +2937,16 @@
         <v>9</v>
       </c>
       <c r="D87" s="2">
-        <v>866.9</v>
+        <v>995</v>
       </c>
       <c r="E87" s="2">
-        <v>113.67282</v>
+        <v>-3.7124999999999999</v>
       </c>
       <c r="F87" s="2">
-        <v>1190.6764900000001</v>
+        <v>3531.8861000000002</v>
       </c>
       <c r="G87" s="2">
-        <v>1319.4387400000001</v>
+        <v>4212.0260200000002</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3035,7 +3020,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>187</v>
       </c>
       <c r="B91" t="s">
         <v>8</v>
@@ -3058,7 +3043,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B92" t="s">
         <v>8</v>
@@ -3081,7 +3066,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>192</v>
+        <v>94</v>
       </c>
       <c r="B93" t="s">
         <v>8</v>
@@ -3113,16 +3098,16 @@
         <v>9</v>
       </c>
       <c r="D94" s="2">
-        <v>995</v>
+        <v>651.74</v>
       </c>
       <c r="E94" s="2">
-        <v>-3.7124999999999999</v>
+        <v>41.505130000000001</v>
       </c>
       <c r="F94" s="2">
-        <v>3531.8861000000002</v>
+        <v>877.23563000000001</v>
       </c>
       <c r="G94" s="2">
-        <v>4212.0260200000002</v>
+        <v>948.54510000000005</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3136,16 +3121,16 @@
         <v>9</v>
       </c>
       <c r="D95" s="2">
-        <v>995</v>
+        <v>656.52</v>
       </c>
       <c r="E95" s="2">
-        <v>-3.7124999999999999</v>
+        <v>52.101509999999998</v>
       </c>
       <c r="F95" s="2">
-        <v>3531.8861000000002</v>
+        <v>1028.4509599999999</v>
       </c>
       <c r="G95" s="2">
-        <v>4212.0260200000002</v>
+        <v>1108.44949</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -3159,16 +3144,16 @@
         <v>9</v>
       </c>
       <c r="D96" s="2">
-        <v>651.74</v>
+        <v>900.53</v>
       </c>
       <c r="E96" s="2">
-        <v>41.505130000000001</v>
+        <v>147.82172</v>
       </c>
       <c r="F96" s="2">
-        <v>877.23563000000001</v>
+        <v>872.92118000000005</v>
       </c>
       <c r="G96" s="2">
-        <v>948.54510000000005</v>
+        <v>873.38602000000003</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -3182,16 +3167,16 @@
         <v>9</v>
       </c>
       <c r="D97" s="2">
-        <v>656.52</v>
+        <v>890.58</v>
       </c>
       <c r="E97" s="2">
-        <v>52.101509999999998</v>
+        <v>118.35751999999999</v>
       </c>
       <c r="F97" s="2">
-        <v>1028.4509599999999</v>
+        <v>779.43859999999995</v>
       </c>
       <c r="G97" s="2">
-        <v>1108.44949</v>
+        <v>754.78877</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3205,16 +3190,16 @@
         <v>9</v>
       </c>
       <c r="D98" s="2">
-        <v>900.53</v>
+        <v>885.46</v>
       </c>
       <c r="E98" s="2">
-        <v>147.82172</v>
+        <v>97.330389999999994</v>
       </c>
       <c r="F98" s="2">
-        <v>872.92118000000005</v>
+        <v>689.04399999999998</v>
       </c>
       <c r="G98" s="2">
-        <v>873.38602000000003</v>
+        <v>641.54237000000001</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3222,68 +3207,68 @@
         <v>100</v>
       </c>
       <c r="B99" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="C99" t="s">
         <v>9</v>
       </c>
       <c r="D99" s="2">
-        <v>890.58</v>
+        <v>322.33</v>
       </c>
       <c r="E99" s="2">
-        <v>118.35751999999999</v>
+        <v>69.377330000000001</v>
       </c>
       <c r="F99" s="2">
-        <v>779.43859999999995</v>
+        <v>1078.9416200000001</v>
       </c>
       <c r="G99" s="2">
-        <v>754.78877</v>
+        <v>1193.5331100000001</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="C100" t="s">
         <v>9</v>
       </c>
       <c r="D100" s="2">
-        <v>885.46</v>
+        <v>220</v>
       </c>
       <c r="E100" s="2">
-        <v>97.330389999999994</v>
+        <v>69.508240000000001</v>
       </c>
       <c r="F100" s="2">
-        <v>689.04399999999998</v>
+        <v>1024.97696</v>
       </c>
       <c r="G100" s="2">
-        <v>641.54237000000001</v>
+        <v>1106.4743699999999</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B101" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C101" t="s">
         <v>9</v>
       </c>
       <c r="D101" s="2">
-        <v>322.33</v>
+        <v>202.46</v>
       </c>
       <c r="E101" s="2">
-        <v>69.377330000000001</v>
+        <v>84.502009999999999</v>
       </c>
       <c r="F101" s="2">
-        <v>1078.9416200000001</v>
+        <v>1096.7771399999999</v>
       </c>
       <c r="G101" s="2">
-        <v>1193.5331100000001</v>
+        <v>1207.3726099999999</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3291,22 +3276,22 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C102" t="s">
         <v>9</v>
       </c>
       <c r="D102" s="2">
-        <v>220</v>
+        <v>863</v>
       </c>
       <c r="E102" s="2">
-        <v>69.508240000000001</v>
+        <v>41.88796</v>
       </c>
       <c r="F102" s="2">
-        <v>1024.97696</v>
+        <v>640.69884999999999</v>
       </c>
       <c r="G102" s="2">
-        <v>1106.4743699999999</v>
+        <v>602.48701000000005</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3314,22 +3299,22 @@
         <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C103" t="s">
         <v>9</v>
       </c>
       <c r="D103" s="2">
-        <v>202.46</v>
+        <v>840</v>
       </c>
       <c r="E103" s="2">
-        <v>84.502009999999999</v>
+        <v>24.30444</v>
       </c>
       <c r="F103" s="2">
-        <v>1096.7771399999999</v>
+        <v>553.62972000000002</v>
       </c>
       <c r="G103" s="2">
-        <v>1207.3726099999999</v>
+        <v>487.09294</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3337,22 +3322,22 @@
         <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C104" t="s">
         <v>9</v>
       </c>
       <c r="D104" s="2">
-        <v>863</v>
+        <v>227.33</v>
       </c>
       <c r="E104" s="2">
-        <v>41.88796</v>
+        <v>29.077290000000001</v>
       </c>
       <c r="F104" s="2">
-        <v>640.69884999999999</v>
+        <v>663.34577999999999</v>
       </c>
       <c r="G104" s="2">
-        <v>602.48701000000005</v>
+        <v>640.21167000000003</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3360,22 +3345,22 @@
         <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C105" t="s">
         <v>9</v>
       </c>
       <c r="D105" s="2">
-        <v>840</v>
+        <v>180</v>
       </c>
       <c r="E105" s="2">
-        <v>24.30444</v>
+        <v>78.419510000000002</v>
       </c>
       <c r="F105" s="2">
-        <v>553.62972000000002</v>
+        <v>822.15782000000002</v>
       </c>
       <c r="G105" s="2">
-        <v>487.09294</v>
+        <v>822.48852999999997</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3383,22 +3368,22 @@
         <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C106" t="s">
         <v>9</v>
       </c>
       <c r="D106" s="2">
-        <v>227.33</v>
+        <v>709.83</v>
       </c>
       <c r="E106" s="2">
-        <v>29.077290000000001</v>
+        <v>31.104130000000001</v>
       </c>
       <c r="F106" s="2">
-        <v>663.34577999999999</v>
+        <v>522.51836000000003</v>
       </c>
       <c r="G106" s="2">
-        <v>640.21167000000003</v>
+        <v>456.98750000000001</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3406,22 +3391,22 @@
         <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C107" t="s">
         <v>9</v>
       </c>
       <c r="D107" s="2">
-        <v>180</v>
+        <v>324.67</v>
       </c>
       <c r="E107" s="2">
-        <v>78.419510000000002</v>
+        <v>38.40016</v>
       </c>
       <c r="F107" s="2">
-        <v>822.15782000000002</v>
+        <v>793.76701000000003</v>
       </c>
       <c r="G107" s="2">
-        <v>822.48852999999997</v>
+        <v>792.19101000000001</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3429,22 +3414,22 @@
         <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C108" t="s">
         <v>9</v>
       </c>
       <c r="D108" s="2">
-        <v>709.83</v>
+        <v>883.51</v>
       </c>
       <c r="E108" s="2">
-        <v>31.104130000000001</v>
+        <v>0.29937999999999998</v>
       </c>
       <c r="F108" s="2">
-        <v>522.51836000000003</v>
+        <v>520.59383000000003</v>
       </c>
       <c r="G108" s="2">
-        <v>456.98750000000001</v>
+        <v>449.67964000000001</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -3452,22 +3437,22 @@
         <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C109" t="s">
         <v>9</v>
       </c>
       <c r="D109" s="2">
-        <v>324.67</v>
+        <v>888.79</v>
       </c>
       <c r="E109" s="2">
-        <v>38.40016</v>
+        <v>80.246449999999996</v>
       </c>
       <c r="F109" s="2">
-        <v>793.76701000000003</v>
+        <v>886.42316000000005</v>
       </c>
       <c r="G109" s="2">
-        <v>792.19101000000001</v>
+        <v>913.66432999999995</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -3475,22 +3460,22 @@
         <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C110" t="s">
         <v>9</v>
       </c>
       <c r="D110" s="2">
-        <v>883.51</v>
+        <v>165</v>
       </c>
       <c r="E110" s="2">
-        <v>0.29937999999999998</v>
+        <v>97.501549999999995</v>
       </c>
       <c r="F110" s="2">
-        <v>520.59383000000003</v>
+        <v>1009.33542</v>
       </c>
       <c r="G110" s="2">
-        <v>449.67964000000001</v>
+        <v>1069.6439600000001</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -3498,22 +3483,22 @@
         <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C111" t="s">
         <v>9</v>
       </c>
       <c r="D111" s="2">
-        <v>888.79</v>
+        <v>165</v>
       </c>
       <c r="E111" s="2">
-        <v>80.246449999999996</v>
+        <v>90.594830000000002</v>
       </c>
       <c r="F111" s="2">
-        <v>886.42316000000005</v>
+        <v>991.28566000000001</v>
       </c>
       <c r="G111" s="2">
-        <v>913.66432999999995</v>
+        <v>1047.25125</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -3521,7 +3506,7 @@
         <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C112" t="s">
         <v>9</v>
@@ -3530,13 +3515,13 @@
         <v>165</v>
       </c>
       <c r="E112" s="2">
-        <v>97.501549999999995</v>
+        <v>98.183639999999997</v>
       </c>
       <c r="F112" s="2">
-        <v>1009.33542</v>
+        <v>1015.74086</v>
       </c>
       <c r="G112" s="2">
-        <v>1069.6439600000001</v>
+        <v>1078.1055799999999</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3544,7 +3529,7 @@
         <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C113" t="s">
         <v>9</v>
@@ -3553,13 +3538,13 @@
         <v>165</v>
       </c>
       <c r="E113" s="2">
-        <v>90.594830000000002</v>
+        <v>91.865719999999996</v>
       </c>
       <c r="F113" s="2">
-        <v>991.28566000000001</v>
+        <v>975.32438000000002</v>
       </c>
       <c r="G113" s="2">
-        <v>1047.25125</v>
+        <v>1030.0664400000001</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -3567,7 +3552,7 @@
         <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C114" t="s">
         <v>9</v>
@@ -3576,13 +3561,13 @@
         <v>165</v>
       </c>
       <c r="E114" s="2">
-        <v>98.183639999999997</v>
+        <v>89.193200000000004</v>
       </c>
       <c r="F114" s="2">
-        <v>1015.74086</v>
+        <v>952.93786</v>
       </c>
       <c r="G114" s="2">
-        <v>1078.1055799999999</v>
+        <v>1000.12405</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3590,7 +3575,7 @@
         <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C115" t="s">
         <v>9</v>
@@ -3599,13 +3584,13 @@
         <v>165</v>
       </c>
       <c r="E115" s="2">
-        <v>91.865719999999996</v>
+        <v>95.571479999999994</v>
       </c>
       <c r="F115" s="2">
-        <v>975.32438000000002</v>
+        <v>987.57272999999998</v>
       </c>
       <c r="G115" s="2">
-        <v>1030.0664400000001</v>
+        <v>1041.9241500000001</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -3613,7 +3598,7 @@
         <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C116" t="s">
         <v>9</v>
@@ -3622,13 +3607,13 @@
         <v>165</v>
       </c>
       <c r="E116" s="2">
-        <v>89.193200000000004</v>
+        <v>83.139060000000001</v>
       </c>
       <c r="F116" s="2">
-        <v>952.93786</v>
+        <v>971.94101999999998</v>
       </c>
       <c r="G116" s="2">
-        <v>1000.12405</v>
+        <v>1030.2670000000001</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -3636,7 +3621,7 @@
         <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C117" t="s">
         <v>9</v>
@@ -3645,13 +3630,13 @@
         <v>165</v>
       </c>
       <c r="E117" s="2">
-        <v>95.571479999999994</v>
+        <v>86.960380000000001</v>
       </c>
       <c r="F117" s="2">
-        <v>987.57272999999998</v>
+        <v>949.41907000000003</v>
       </c>
       <c r="G117" s="2">
-        <v>1041.9241500000001</v>
+        <v>997.13861999999995</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -3659,7 +3644,7 @@
         <v>120</v>
       </c>
       <c r="B118" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C118" t="s">
         <v>9</v>
@@ -3668,13 +3653,13 @@
         <v>165</v>
       </c>
       <c r="E118" s="2">
-        <v>83.139060000000001</v>
+        <v>92.871740000000003</v>
       </c>
       <c r="F118" s="2">
-        <v>971.94101999999998</v>
+        <v>985.42692999999997</v>
       </c>
       <c r="G118" s="2">
-        <v>1030.2670000000001</v>
+        <v>1040.4312600000001</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -3682,7 +3667,7 @@
         <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C119" t="s">
         <v>9</v>
@@ -3691,13 +3676,13 @@
         <v>165</v>
       </c>
       <c r="E119" s="2">
-        <v>86.960380000000001</v>
+        <v>91.728039999999993</v>
       </c>
       <c r="F119" s="2">
-        <v>949.41907000000003</v>
+        <v>980.80745999999999</v>
       </c>
       <c r="G119" s="2">
-        <v>997.13861999999995</v>
+        <v>1035.51856</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -3705,22 +3690,22 @@
         <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C120" t="s">
         <v>9</v>
       </c>
       <c r="D120" s="2">
-        <v>165</v>
+        <v>370</v>
       </c>
       <c r="E120" s="2">
-        <v>92.871740000000003</v>
+        <v>46.593539999999997</v>
       </c>
       <c r="F120" s="2">
-        <v>985.42692999999997</v>
+        <v>717.65364</v>
       </c>
       <c r="G120" s="2">
-        <v>1040.4312600000001</v>
+        <v>697.20482000000004</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -3728,22 +3713,22 @@
         <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C121" t="s">
         <v>9</v>
       </c>
       <c r="D121" s="2">
-        <v>165</v>
+        <v>456</v>
       </c>
       <c r="E121" s="2">
-        <v>91.728039999999993</v>
+        <v>55.974530000000001</v>
       </c>
       <c r="F121" s="2">
-        <v>980.80745999999999</v>
+        <v>803.01868999999999</v>
       </c>
       <c r="G121" s="2">
-        <v>1035.51856</v>
+        <v>806.94732999999997</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -3751,22 +3736,22 @@
         <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C122" t="s">
         <v>9</v>
       </c>
       <c r="D122" s="2">
-        <v>370</v>
+        <v>845</v>
       </c>
       <c r="E122" s="2">
-        <v>46.593539999999997</v>
+        <v>36.930439999999997</v>
       </c>
       <c r="F122" s="2">
-        <v>717.65364</v>
+        <v>698.16184999999996</v>
       </c>
       <c r="G122" s="2">
-        <v>697.20482000000004</v>
+        <v>669.85233000000005</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -3774,22 +3759,22 @@
         <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C123" t="s">
         <v>9</v>
       </c>
       <c r="D123" s="2">
-        <v>456</v>
+        <v>845</v>
       </c>
       <c r="E123" s="2">
-        <v>55.974530000000001</v>
+        <v>55.620109999999997</v>
       </c>
       <c r="F123" s="2">
-        <v>803.01868999999999</v>
+        <v>756.23338000000001</v>
       </c>
       <c r="G123" s="2">
-        <v>806.94732999999997</v>
+        <v>745.82642999999996</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -3797,7 +3782,7 @@
         <v>126</v>
       </c>
       <c r="B124" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C124" t="s">
         <v>9</v>
@@ -3806,13 +3791,13 @@
         <v>845</v>
       </c>
       <c r="E124" s="2">
-        <v>36.930439999999997</v>
+        <v>73.029470000000003</v>
       </c>
       <c r="F124" s="2">
-        <v>698.16184999999996</v>
+        <v>834.62203</v>
       </c>
       <c r="G124" s="2">
-        <v>669.85233000000005</v>
+        <v>847.61706000000004</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -3820,22 +3805,22 @@
         <v>127</v>
       </c>
       <c r="B125" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C125" t="s">
         <v>9</v>
       </c>
       <c r="D125" s="2">
-        <v>845</v>
+        <v>450</v>
       </c>
       <c r="E125" s="2">
-        <v>55.620109999999997</v>
+        <v>66.173749999999998</v>
       </c>
       <c r="F125" s="2">
-        <v>756.23338000000001</v>
+        <v>945.36153999999999</v>
       </c>
       <c r="G125" s="2">
-        <v>745.82642999999996</v>
+        <v>987.39417000000003</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -3843,22 +3828,22 @@
         <v>128</v>
       </c>
       <c r="B126" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C126" t="s">
         <v>9</v>
       </c>
       <c r="D126" s="2">
-        <v>845</v>
+        <v>450</v>
       </c>
       <c r="E126" s="2">
-        <v>73.029470000000003</v>
+        <v>62.140500000000003</v>
       </c>
       <c r="F126" s="2">
-        <v>834.62203</v>
+        <v>931.12222999999994</v>
       </c>
       <c r="G126" s="2">
-        <v>847.61706000000004</v>
+        <v>967.78536999999994</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -3866,7 +3851,7 @@
         <v>129</v>
       </c>
       <c r="B127" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C127" t="s">
         <v>9</v>
@@ -3875,13 +3860,13 @@
         <v>450</v>
       </c>
       <c r="E127" s="2">
-        <v>66.173749999999998</v>
+        <v>69.110259999999997</v>
       </c>
       <c r="F127" s="2">
-        <v>945.36153999999999</v>
+        <v>956.01424999999995</v>
       </c>
       <c r="G127" s="2">
-        <v>987.39417000000003</v>
+        <v>999.45385999999996</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -3889,7 +3874,7 @@
         <v>130</v>
       </c>
       <c r="B128" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C128" t="s">
         <v>9</v>
@@ -3898,13 +3883,13 @@
         <v>450</v>
       </c>
       <c r="E128" s="2">
-        <v>62.140500000000003</v>
+        <v>58.532800000000002</v>
       </c>
       <c r="F128" s="2">
-        <v>931.12222999999994</v>
+        <v>920.14088000000004</v>
       </c>
       <c r="G128" s="2">
-        <v>967.78536999999994</v>
+        <v>955.99950999999999</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -3912,7 +3897,7 @@
         <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C129" t="s">
         <v>9</v>
@@ -3921,13 +3906,13 @@
         <v>450</v>
       </c>
       <c r="E129" s="2">
-        <v>69.110259999999997</v>
+        <v>54.38843</v>
       </c>
       <c r="F129" s="2">
-        <v>956.01424999999995</v>
+        <v>901.95781999999997</v>
       </c>
       <c r="G129" s="2">
-        <v>999.45385999999996</v>
+        <v>931.05181000000005</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -3935,7 +3920,7 @@
         <v>132</v>
       </c>
       <c r="B130" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C130" t="s">
         <v>9</v>
@@ -3944,13 +3929,13 @@
         <v>450</v>
       </c>
       <c r="E130" s="2">
-        <v>58.532800000000002</v>
+        <v>61.56765</v>
       </c>
       <c r="F130" s="2">
-        <v>920.14088000000004</v>
+        <v>933.38172999999995</v>
       </c>
       <c r="G130" s="2">
-        <v>955.99950999999999</v>
+        <v>969.31545000000006</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -3958,7 +3943,7 @@
         <v>133</v>
       </c>
       <c r="B131" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C131" t="s">
         <v>9</v>
@@ -3967,13 +3952,13 @@
         <v>450</v>
       </c>
       <c r="E131" s="2">
-        <v>54.38843</v>
+        <v>64.756900000000002</v>
       </c>
       <c r="F131" s="2">
-        <v>901.95781999999997</v>
+        <v>924.11273000000006</v>
       </c>
       <c r="G131" s="2">
-        <v>931.05181000000005</v>
+        <v>966.42352000000005</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -3981,7 +3966,7 @@
         <v>134</v>
       </c>
       <c r="B132" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C132" t="s">
         <v>9</v>
@@ -3990,13 +3975,13 @@
         <v>450</v>
       </c>
       <c r="E132" s="2">
-        <v>61.56765</v>
+        <v>63.789879999999997</v>
       </c>
       <c r="F132" s="2">
-        <v>933.38172999999995</v>
+        <v>914.83558000000005</v>
       </c>
       <c r="G132" s="2">
-        <v>969.31545000000006</v>
+        <v>951.97581000000002</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -4004,7 +3989,7 @@
         <v>135</v>
       </c>
       <c r="B133" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C133" t="s">
         <v>9</v>
@@ -4013,13 +3998,13 @@
         <v>450</v>
       </c>
       <c r="E133" s="2">
-        <v>64.756900000000002</v>
+        <v>68.381600000000006</v>
       </c>
       <c r="F133" s="2">
-        <v>924.11273000000006</v>
+        <v>943.88905999999997</v>
       </c>
       <c r="G133" s="2">
-        <v>966.42352000000005</v>
+        <v>987.58330999999998</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -4027,7 +4012,7 @@
         <v>136</v>
       </c>
       <c r="B134" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C134" t="s">
         <v>9</v>
@@ -4036,13 +4021,13 @@
         <v>450</v>
       </c>
       <c r="E134" s="2">
-        <v>63.789879999999997</v>
+        <v>63.417639999999999</v>
       </c>
       <c r="F134" s="2">
-        <v>914.83558000000005</v>
+        <v>929.11897999999997</v>
       </c>
       <c r="G134" s="2">
-        <v>951.97581000000002</v>
+        <v>967.71463000000006</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -4050,22 +4035,22 @@
         <v>137</v>
       </c>
       <c r="B135" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C135" t="s">
         <v>9</v>
       </c>
       <c r="D135" s="2">
-        <v>450</v>
+        <v>840</v>
       </c>
       <c r="E135" s="2">
-        <v>68.381600000000006</v>
+        <v>-0.82150000000000001</v>
       </c>
       <c r="F135" s="2">
-        <v>943.88905999999997</v>
+        <v>531.07858999999996</v>
       </c>
       <c r="G135" s="2">
-        <v>987.58330999999998</v>
+        <v>462.90652999999998</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -4073,22 +4058,22 @@
         <v>138</v>
       </c>
       <c r="B136" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C136" t="s">
         <v>9</v>
       </c>
       <c r="D136" s="2">
-        <v>450</v>
+        <v>830</v>
       </c>
       <c r="E136" s="2">
-        <v>63.417639999999999</v>
+        <v>71.182540000000003</v>
       </c>
       <c r="F136" s="2">
-        <v>929.11897999999997</v>
+        <v>649.30093999999997</v>
       </c>
       <c r="G136" s="2">
-        <v>967.71463000000006</v>
+        <v>602.11006999999995</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -4096,22 +4081,22 @@
         <v>139</v>
       </c>
       <c r="B137" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C137" t="s">
         <v>9</v>
       </c>
       <c r="D137" s="2">
-        <v>840</v>
+        <v>364.08</v>
       </c>
       <c r="E137" s="2">
-        <v>-0.82150000000000001</v>
+        <v>38.198630000000001</v>
       </c>
       <c r="F137" s="2">
-        <v>531.07858999999996</v>
+        <v>671.97681999999998</v>
       </c>
       <c r="G137" s="2">
-        <v>462.90652999999998</v>
+        <v>642.83272999999997</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -4119,22 +4104,22 @@
         <v>140</v>
       </c>
       <c r="B138" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C138" t="s">
         <v>9</v>
       </c>
       <c r="D138" s="2">
-        <v>830</v>
+        <v>898.54</v>
       </c>
       <c r="E138" s="2">
-        <v>71.182540000000003</v>
+        <v>80.59187</v>
       </c>
       <c r="F138" s="2">
-        <v>649.30093999999997</v>
+        <v>784.49432999999999</v>
       </c>
       <c r="G138" s="2">
-        <v>602.11006999999995</v>
+        <v>779.01937999999996</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -4142,22 +4127,22 @@
         <v>141</v>
       </c>
       <c r="B139" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C139" t="s">
         <v>9</v>
       </c>
       <c r="D139" s="2">
-        <v>364.08</v>
+        <v>830</v>
       </c>
       <c r="E139" s="2">
-        <v>38.198630000000001</v>
+        <v>24.505520000000001</v>
       </c>
       <c r="F139" s="2">
-        <v>671.97681999999998</v>
+        <v>445.31778000000003</v>
       </c>
       <c r="G139" s="2">
-        <v>642.83272999999997</v>
+        <v>356.71605</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -4165,22 +4150,22 @@
         <v>142</v>
       </c>
       <c r="B140" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C140" t="s">
         <v>9</v>
       </c>
       <c r="D140" s="2">
-        <v>898.54</v>
+        <v>130</v>
       </c>
       <c r="E140" s="2">
-        <v>80.59187</v>
+        <v>95.399959999999993</v>
       </c>
       <c r="F140" s="2">
-        <v>784.49432999999999</v>
+        <v>822.21927000000005</v>
       </c>
       <c r="G140" s="2">
-        <v>779.01937999999996</v>
+        <v>826.97820999999999</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -4188,22 +4173,22 @@
         <v>143</v>
       </c>
       <c r="B141" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C141" t="s">
         <v>9</v>
       </c>
       <c r="D141" s="2">
-        <v>830</v>
+        <v>872.24</v>
       </c>
       <c r="E141" s="2">
-        <v>24.505520000000001</v>
+        <v>74.514300000000006</v>
       </c>
       <c r="F141" s="2">
-        <v>445.31778000000003</v>
+        <v>663.13103000000001</v>
       </c>
       <c r="G141" s="2">
-        <v>356.71605</v>
+        <v>624.61014</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -4211,22 +4196,22 @@
         <v>144</v>
       </c>
       <c r="B142" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C142" t="s">
         <v>9</v>
       </c>
       <c r="D142" s="2">
-        <v>130</v>
+        <v>403.1</v>
       </c>
       <c r="E142" s="2">
-        <v>95.399959999999993</v>
+        <v>37.935870000000001</v>
       </c>
       <c r="F142" s="2">
-        <v>822.21927000000005</v>
+        <v>677.81901000000005</v>
       </c>
       <c r="G142" s="2">
-        <v>826.97820999999999</v>
+        <v>650.34451999999999</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -4234,22 +4219,22 @@
         <v>145</v>
       </c>
       <c r="B143" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C143" t="s">
         <v>9</v>
       </c>
       <c r="D143" s="2">
-        <v>872.24</v>
+        <v>902.56</v>
       </c>
       <c r="E143" s="2">
-        <v>74.514300000000006</v>
+        <v>73.277169999999998</v>
       </c>
       <c r="F143" s="2">
-        <v>663.13103000000001</v>
+        <v>670.87559999999996</v>
       </c>
       <c r="G143" s="2">
-        <v>624.61014</v>
+        <v>637.03657999999996</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -4257,91 +4242,91 @@
         <v>146</v>
       </c>
       <c r="B144" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C144" t="s">
         <v>9</v>
       </c>
       <c r="D144" s="2">
-        <v>403.1</v>
+        <v>201</v>
       </c>
       <c r="E144" s="2">
-        <v>37.935870000000001</v>
+        <v>41.472200000000001</v>
       </c>
       <c r="F144" s="2">
-        <v>677.81901000000005</v>
+        <v>827.30825000000004</v>
       </c>
       <c r="G144" s="2">
-        <v>650.34451999999999</v>
+        <v>833.82885999999996</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>147</v>
+        <v>188</v>
       </c>
       <c r="B145" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C145" t="s">
         <v>9</v>
       </c>
       <c r="D145" s="2">
-        <v>902.56</v>
+        <v>849</v>
       </c>
       <c r="E145" s="2">
-        <v>73.277169999999998</v>
+        <v>-13.898250000000001</v>
       </c>
       <c r="F145" s="2">
-        <v>670.87559999999996</v>
+        <v>327.42838</v>
       </c>
       <c r="G145" s="2">
-        <v>637.03657999999996</v>
+        <v>232.10374999999999</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B146" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C146" t="s">
         <v>9</v>
       </c>
       <c r="D146" s="2">
-        <v>201</v>
+        <v>840</v>
       </c>
       <c r="E146" s="2">
-        <v>41.472200000000001</v>
+        <v>-7.8560800000000004</v>
       </c>
       <c r="F146" s="2">
-        <v>827.30825000000004</v>
+        <v>481.86457000000001</v>
       </c>
       <c r="G146" s="2">
-        <v>833.82885999999996</v>
+        <v>404.23880000000003</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>193</v>
+        <v>148</v>
       </c>
       <c r="B147" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C147" t="s">
         <v>9</v>
       </c>
       <c r="D147" s="2">
-        <v>849</v>
+        <v>250</v>
       </c>
       <c r="E147" s="2">
-        <v>-13.898250000000001</v>
+        <v>46.257330000000003</v>
       </c>
       <c r="F147" s="2">
-        <v>327.42838</v>
+        <v>945.21835999999996</v>
       </c>
       <c r="G147" s="2">
-        <v>232.10374999999999</v>
+        <v>989.66785000000004</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -4349,22 +4334,22 @@
         <v>149</v>
       </c>
       <c r="B148" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C148" t="s">
         <v>9</v>
       </c>
       <c r="D148" s="2">
-        <v>840</v>
+        <v>160</v>
       </c>
       <c r="E148" s="2">
-        <v>-7.8560800000000004</v>
+        <v>60.384349999999998</v>
       </c>
       <c r="F148" s="2">
-        <v>481.86457000000001</v>
+        <v>912.69644000000005</v>
       </c>
       <c r="G148" s="2">
-        <v>404.23880000000003</v>
+        <v>945.67197999999996</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -4372,22 +4357,22 @@
         <v>150</v>
       </c>
       <c r="B149" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C149" t="s">
         <v>9</v>
       </c>
       <c r="D149" s="2">
-        <v>250</v>
+        <v>435</v>
       </c>
       <c r="E149" s="2">
-        <v>46.257330000000003</v>
+        <v>56.53192</v>
       </c>
       <c r="F149" s="2">
-        <v>945.21835999999996</v>
+        <v>976.37275</v>
       </c>
       <c r="G149" s="2">
-        <v>989.66785000000004</v>
+        <v>1019.13749</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -4395,22 +4380,22 @@
         <v>151</v>
       </c>
       <c r="B150" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C150" t="s">
         <v>9</v>
       </c>
       <c r="D150" s="2">
-        <v>160</v>
+        <v>324</v>
       </c>
       <c r="E150" s="2">
-        <v>60.384349999999998</v>
+        <v>51.145069999999997</v>
       </c>
       <c r="F150" s="2">
-        <v>912.69644000000005</v>
+        <v>940.3374</v>
       </c>
       <c r="G150" s="2">
-        <v>945.67197999999996</v>
+        <v>972.87469999999996</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -4418,22 +4403,22 @@
         <v>152</v>
       </c>
       <c r="B151" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C151" t="s">
         <v>9</v>
       </c>
       <c r="D151" s="2">
-        <v>320</v>
+        <v>361</v>
       </c>
       <c r="E151" s="2">
-        <v>0</v>
+        <v>53.232939999999999</v>
       </c>
       <c r="F151" s="2">
-        <v>0</v>
+        <v>955.65659000000005</v>
       </c>
       <c r="G151" s="2">
-        <v>0</v>
+        <v>992.71022000000005</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -4441,22 +4426,22 @@
         <v>153</v>
       </c>
       <c r="B152" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C152" t="s">
         <v>9</v>
       </c>
       <c r="D152" s="2">
-        <v>435</v>
+        <v>398</v>
       </c>
       <c r="E152" s="2">
-        <v>56.53192</v>
+        <v>54.514499999999998</v>
       </c>
       <c r="F152" s="2">
-        <v>976.37275</v>
+        <v>966.62543000000005</v>
       </c>
       <c r="G152" s="2">
-        <v>1019.13749</v>
+        <v>1006.58323</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -4464,22 +4449,22 @@
         <v>154</v>
       </c>
       <c r="B153" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C153" t="s">
         <v>9</v>
       </c>
       <c r="D153" s="2">
-        <v>324</v>
+        <v>260</v>
       </c>
       <c r="E153" s="2">
-        <v>51.145069999999997</v>
+        <v>77.31532</v>
       </c>
       <c r="F153" s="2">
-        <v>940.3374</v>
+        <v>931.48364000000004</v>
       </c>
       <c r="G153" s="2">
-        <v>972.87469999999996</v>
+        <v>1033.22102</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
@@ -4487,22 +4472,22 @@
         <v>155</v>
       </c>
       <c r="B154" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C154" t="s">
         <v>9</v>
       </c>
       <c r="D154" s="2">
-        <v>361</v>
+        <v>877.82</v>
       </c>
       <c r="E154" s="2">
-        <v>53.232939999999999</v>
+        <v>-4.8858800000000002</v>
       </c>
       <c r="F154" s="2">
-        <v>955.65659000000005</v>
+        <v>425.12484000000001</v>
       </c>
       <c r="G154" s="2">
-        <v>992.71022000000005</v>
+        <v>342.87884000000003</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
@@ -4510,22 +4495,22 @@
         <v>156</v>
       </c>
       <c r="B155" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C155" t="s">
         <v>9</v>
       </c>
       <c r="D155" s="2">
-        <v>398</v>
+        <v>325.83999999999997</v>
       </c>
       <c r="E155" s="2">
-        <v>54.514499999999998</v>
+        <v>46.67989</v>
       </c>
       <c r="F155" s="2">
-        <v>966.62543000000005</v>
+        <v>709.43140000000005</v>
       </c>
       <c r="G155" s="2">
-        <v>1006.58323</v>
+        <v>680.86659999999995</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -4533,22 +4518,22 @@
         <v>157</v>
       </c>
       <c r="B156" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C156" t="s">
         <v>9</v>
       </c>
       <c r="D156" s="2">
-        <v>260</v>
+        <v>139.28</v>
       </c>
       <c r="E156" s="2">
-        <v>77.31532</v>
+        <v>100.95616</v>
       </c>
       <c r="F156" s="2">
-        <v>931.48364000000004</v>
+        <v>1056.0173600000001</v>
       </c>
       <c r="G156" s="2">
-        <v>1033.22102</v>
+        <v>1168.53693</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -4556,22 +4541,22 @@
         <v>158</v>
       </c>
       <c r="B157" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C157" t="s">
         <v>9</v>
       </c>
       <c r="D157" s="2">
-        <v>877.82</v>
+        <v>149</v>
       </c>
       <c r="E157" s="2">
-        <v>-4.8858800000000002</v>
+        <v>76.252560000000003</v>
       </c>
       <c r="F157" s="2">
-        <v>425.12484000000001</v>
+        <v>1025.9431099999999</v>
       </c>
       <c r="G157" s="2">
-        <v>342.87884000000003</v>
+        <v>1121.6369199999999</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -4579,22 +4564,22 @@
         <v>159</v>
       </c>
       <c r="B158" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C158" t="s">
         <v>9</v>
       </c>
       <c r="D158" s="2">
-        <v>325.83999999999997</v>
+        <v>200</v>
       </c>
       <c r="E158" s="2">
-        <v>46.67989</v>
+        <v>82.404269999999997</v>
       </c>
       <c r="F158" s="2">
-        <v>709.43140000000005</v>
+        <v>1109.71505</v>
       </c>
       <c r="G158" s="2">
-        <v>680.86659999999995</v>
+        <v>1239.2553700000001</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -4602,22 +4587,22 @@
         <v>160</v>
       </c>
       <c r="B159" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C159" t="s">
         <v>9</v>
       </c>
       <c r="D159" s="2">
-        <v>139.28</v>
+        <v>112.25</v>
       </c>
       <c r="E159" s="2">
-        <v>100.95616</v>
+        <v>93.868009999999998</v>
       </c>
       <c r="F159" s="2">
-        <v>1056.0173600000001</v>
+        <v>1071.49451</v>
       </c>
       <c r="G159" s="2">
-        <v>1168.53693</v>
+        <v>1181.5035</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -4625,22 +4610,22 @@
         <v>161</v>
       </c>
       <c r="B160" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C160" t="s">
         <v>9</v>
       </c>
       <c r="D160" s="2">
-        <v>149</v>
+        <v>183.52</v>
       </c>
       <c r="E160" s="2">
-        <v>76.252560000000003</v>
+        <v>36.497619999999998</v>
       </c>
       <c r="F160" s="2">
-        <v>1025.9431099999999</v>
+        <v>803.10267999999996</v>
       </c>
       <c r="G160" s="2">
-        <v>1121.6369199999999</v>
+        <v>804.52413999999999</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -4648,91 +4633,91 @@
         <v>162</v>
       </c>
       <c r="B161" t="s">
-        <v>103</v>
+        <v>163</v>
       </c>
       <c r="C161" t="s">
         <v>9</v>
       </c>
       <c r="D161" s="2">
-        <v>200</v>
+        <v>161.41</v>
       </c>
       <c r="E161" s="2">
-        <v>82.404269999999997</v>
+        <v>90.522919999999999</v>
       </c>
       <c r="F161" s="2">
-        <v>1109.71505</v>
+        <v>1030.8917200000001</v>
       </c>
       <c r="G161" s="2">
-        <v>1239.2553700000001</v>
+        <v>1108.0258799999999</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
+        <v>164</v>
+      </c>
+      <c r="B162" t="s">
         <v>163</v>
       </c>
-      <c r="B162" t="s">
-        <v>103</v>
-      </c>
       <c r="C162" t="s">
         <v>9</v>
       </c>
       <c r="D162" s="2">
-        <v>112.25</v>
+        <v>212</v>
       </c>
       <c r="E162" s="2">
-        <v>93.868009999999998</v>
+        <v>83.934359999999998</v>
       </c>
       <c r="F162" s="2">
-        <v>1071.49451</v>
+        <v>1128.33917</v>
       </c>
       <c r="G162" s="2">
-        <v>1181.5035</v>
+        <v>1247.0399</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B163" t="s">
-        <v>103</v>
+        <v>163</v>
       </c>
       <c r="C163" t="s">
         <v>9</v>
       </c>
       <c r="D163" s="2">
-        <v>183.52</v>
+        <v>118.5</v>
       </c>
       <c r="E163" s="2">
-        <v>36.497619999999998</v>
+        <v>114.98211999999999</v>
       </c>
       <c r="F163" s="2">
-        <v>803.10267999999996</v>
+        <v>1082.2521999999999</v>
       </c>
       <c r="G163" s="2">
-        <v>804.52413999999999</v>
+        <v>1183.81287</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B164" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C164" t="s">
         <v>9</v>
       </c>
       <c r="D164" s="2">
-        <v>161.41</v>
+        <v>156.69999999999999</v>
       </c>
       <c r="E164" s="2">
-        <v>90.522919999999999</v>
+        <v>124.76308</v>
       </c>
       <c r="F164" s="2">
-        <v>1030.8917200000001</v>
+        <v>1113.4349999999999</v>
       </c>
       <c r="G164" s="2">
-        <v>1108.0258799999999</v>
+        <v>1228.17552</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
@@ -4740,22 +4725,22 @@
         <v>167</v>
       </c>
       <c r="B165" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C165" t="s">
         <v>9</v>
       </c>
       <c r="D165" s="2">
-        <v>212</v>
+        <v>138.30000000000001</v>
       </c>
       <c r="E165" s="2">
-        <v>83.934359999999998</v>
+        <v>119.56726999999999</v>
       </c>
       <c r="F165" s="2">
-        <v>1128.33917</v>
+        <v>1096.7928400000001</v>
       </c>
       <c r="G165" s="2">
-        <v>1247.0399</v>
+        <v>1203.7130299999999</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -4763,22 +4748,22 @@
         <v>168</v>
       </c>
       <c r="B166" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C166" t="s">
         <v>9</v>
       </c>
       <c r="D166" s="2">
-        <v>118.5</v>
+        <v>145</v>
       </c>
       <c r="E166" s="2">
-        <v>114.98211999999999</v>
+        <v>122.19844999999999</v>
       </c>
       <c r="F166" s="2">
-        <v>1082.2521999999999</v>
+        <v>1108.9523099999999</v>
       </c>
       <c r="G166" s="2">
-        <v>1183.81287</v>
+        <v>1221.19759</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -4786,22 +4771,22 @@
         <v>169</v>
       </c>
       <c r="B167" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C167" t="s">
         <v>9</v>
       </c>
       <c r="D167" s="2">
-        <v>156.69999999999999</v>
+        <v>258.11</v>
       </c>
       <c r="E167" s="2">
-        <v>124.76308</v>
+        <v>146.54954000000001</v>
       </c>
       <c r="F167" s="2">
-        <v>1113.4349999999999</v>
+        <v>946.67961000000003</v>
       </c>
       <c r="G167" s="2">
-        <v>1228.17552</v>
+        <v>952.40196000000003</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -4809,22 +4794,22 @@
         <v>170</v>
       </c>
       <c r="B168" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C168" t="s">
         <v>9</v>
       </c>
       <c r="D168" s="2">
-        <v>138.30000000000001</v>
+        <v>222</v>
       </c>
       <c r="E168" s="2">
-        <v>119.56726999999999</v>
+        <v>137.33089000000001</v>
       </c>
       <c r="F168" s="2">
-        <v>1096.7928400000001</v>
+        <v>944.80776000000003</v>
       </c>
       <c r="G168" s="2">
-        <v>1203.7130299999999</v>
+        <v>951.34226000000001</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -4832,22 +4817,22 @@
         <v>171</v>
       </c>
       <c r="B169" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C169" t="s">
         <v>9</v>
       </c>
       <c r="D169" s="2">
-        <v>145</v>
+        <v>265</v>
       </c>
       <c r="E169" s="2">
-        <v>122.19844999999999</v>
+        <v>140.16818000000001</v>
       </c>
       <c r="F169" s="2">
-        <v>1108.9523099999999</v>
+        <v>941.21596</v>
       </c>
       <c r="G169" s="2">
-        <v>1221.19759</v>
+        <v>946.75824</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
@@ -4855,22 +4840,22 @@
         <v>172</v>
       </c>
       <c r="B170" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C170" t="s">
         <v>9</v>
       </c>
       <c r="D170" s="2">
-        <v>258.11</v>
+        <v>248</v>
       </c>
       <c r="E170" s="2">
-        <v>146.54954000000001</v>
+        <v>94.743579999999994</v>
       </c>
       <c r="F170" s="2">
-        <v>946.67961000000003</v>
+        <v>1067.0728200000001</v>
       </c>
       <c r="G170" s="2">
-        <v>952.40196000000003</v>
+        <v>1164.5875599999999</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -4878,22 +4863,22 @@
         <v>173</v>
       </c>
       <c r="B171" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C171" t="s">
         <v>9</v>
       </c>
       <c r="D171" s="2">
-        <v>222</v>
+        <v>232.07</v>
       </c>
       <c r="E171" s="2">
-        <v>137.33089000000001</v>
+        <v>83.050730000000001</v>
       </c>
       <c r="F171" s="2">
-        <v>944.80776000000003</v>
+        <v>984.83271999999999</v>
       </c>
       <c r="G171" s="2">
-        <v>951.34226000000001</v>
+        <v>1055.1437100000001</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
@@ -4901,22 +4886,22 @@
         <v>174</v>
       </c>
       <c r="B172" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C172" t="s">
         <v>9</v>
       </c>
       <c r="D172" s="2">
-        <v>265</v>
+        <v>632</v>
       </c>
       <c r="E172" s="2">
-        <v>140.16818000000001</v>
+        <v>77.503979999999999</v>
       </c>
       <c r="F172" s="2">
-        <v>941.21596</v>
+        <v>1175.5896299999999</v>
       </c>
       <c r="G172" s="2">
-        <v>946.75824</v>
+        <v>1291.5400500000001</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
@@ -4924,22 +4909,22 @@
         <v>175</v>
       </c>
       <c r="B173" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C173" t="s">
         <v>9</v>
       </c>
       <c r="D173" s="2">
-        <v>248</v>
+        <v>525</v>
       </c>
       <c r="E173" s="2">
-        <v>94.743579999999994</v>
+        <v>75.43262</v>
       </c>
       <c r="F173" s="2">
-        <v>1067.0728200000001</v>
+        <v>1145.64688</v>
       </c>
       <c r="G173" s="2">
-        <v>1164.5875599999999</v>
+        <v>1249.98378</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
@@ -4947,22 +4932,22 @@
         <v>176</v>
       </c>
       <c r="B174" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C174" t="s">
         <v>9</v>
       </c>
       <c r="D174" s="2">
-        <v>232.07</v>
+        <v>662</v>
       </c>
       <c r="E174" s="2">
-        <v>83.050730000000001</v>
+        <v>82.458960000000005</v>
       </c>
       <c r="F174" s="2">
-        <v>984.83271999999999</v>
+        <v>1207.6604299999999</v>
       </c>
       <c r="G174" s="2">
-        <v>1055.1437100000001</v>
+        <v>1333.7865099999999</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -4970,22 +4955,22 @@
         <v>177</v>
       </c>
       <c r="B175" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C175" t="s">
         <v>9</v>
       </c>
       <c r="D175" s="2">
-        <v>632</v>
+        <v>414</v>
       </c>
       <c r="E175" s="2">
-        <v>77.503979999999999</v>
+        <v>89.739720000000005</v>
       </c>
       <c r="F175" s="2">
-        <v>1175.5896299999999</v>
+        <v>1064.1295299999999</v>
       </c>
       <c r="G175" s="2">
-        <v>1291.5400500000001</v>
+        <v>1136.9253699999999</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -4993,22 +4978,22 @@
         <v>178</v>
       </c>
       <c r="B176" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C176" t="s">
         <v>9</v>
       </c>
       <c r="D176" s="2">
-        <v>525</v>
+        <v>418</v>
       </c>
       <c r="E176" s="2">
-        <v>75.43262</v>
+        <v>107.29031000000001</v>
       </c>
       <c r="F176" s="2">
-        <v>1145.64688</v>
+        <v>1099.4960900000001</v>
       </c>
       <c r="G176" s="2">
-        <v>1249.98378</v>
+        <v>1185.8258599999999</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
@@ -5016,22 +5001,22 @@
         <v>179</v>
       </c>
       <c r="B177" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C177" t="s">
         <v>9</v>
       </c>
       <c r="D177" s="2">
-        <v>662</v>
+        <v>259</v>
       </c>
       <c r="E177" s="2">
-        <v>82.458960000000005</v>
+        <v>126.16269</v>
       </c>
       <c r="F177" s="2">
-        <v>1207.6604299999999</v>
+        <v>1196.2801300000001</v>
       </c>
       <c r="G177" s="2">
-        <v>1333.7865099999999</v>
+        <v>1308.4807000000001</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
@@ -5039,22 +5024,22 @@
         <v>180</v>
       </c>
       <c r="B178" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C178" t="s">
         <v>9</v>
       </c>
       <c r="D178" s="2">
-        <v>418</v>
+        <v>261</v>
       </c>
       <c r="E178" s="2">
-        <v>0</v>
+        <v>167.53682000000001</v>
       </c>
       <c r="F178" s="2">
-        <v>0</v>
+        <v>1188.50422</v>
       </c>
       <c r="G178" s="2">
-        <v>0</v>
+        <v>1291.3612499999999</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
@@ -5062,136 +5047,21 @@
         <v>181</v>
       </c>
       <c r="B179" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C179" t="s">
         <v>9</v>
       </c>
       <c r="D179" s="2">
-        <v>414</v>
+        <v>256</v>
       </c>
       <c r="E179" s="2">
-        <v>89.739720000000005</v>
+        <v>137.65004999999999</v>
       </c>
       <c r="F179" s="2">
-        <v>1064.1295299999999</v>
+        <v>1203.25578</v>
       </c>
       <c r="G179" s="2">
-        <v>1136.9253699999999</v>
-      </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>182</v>
-      </c>
-      <c r="B180" t="s">
-        <v>166</v>
-      </c>
-      <c r="C180" t="s">
-        <v>9</v>
-      </c>
-      <c r="D180" s="2">
-        <v>418</v>
-      </c>
-      <c r="E180" s="2">
-        <v>107.29031000000001</v>
-      </c>
-      <c r="F180" s="2">
-        <v>1099.4960900000001</v>
-      </c>
-      <c r="G180" s="2">
-        <v>1185.8258599999999</v>
-      </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>183</v>
-      </c>
-      <c r="B181" t="s">
-        <v>166</v>
-      </c>
-      <c r="C181" t="s">
-        <v>9</v>
-      </c>
-      <c r="D181" s="2">
-        <v>260.38</v>
-      </c>
-      <c r="E181" s="2">
-        <v>0</v>
-      </c>
-      <c r="F181" s="2">
-        <v>0</v>
-      </c>
-      <c r="G181" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>184</v>
-      </c>
-      <c r="B182" t="s">
-        <v>166</v>
-      </c>
-      <c r="C182" t="s">
-        <v>9</v>
-      </c>
-      <c r="D182" s="2">
-        <v>259</v>
-      </c>
-      <c r="E182" s="2">
-        <v>126.16269</v>
-      </c>
-      <c r="F182" s="2">
-        <v>1196.2801300000001</v>
-      </c>
-      <c r="G182" s="2">
-        <v>1308.4807000000001</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>185</v>
-      </c>
-      <c r="B183" t="s">
-        <v>166</v>
-      </c>
-      <c r="C183" t="s">
-        <v>9</v>
-      </c>
-      <c r="D183" s="2">
-        <v>261</v>
-      </c>
-      <c r="E183" s="2">
-        <v>167.53682000000001</v>
-      </c>
-      <c r="F183" s="2">
-        <v>1188.50422</v>
-      </c>
-      <c r="G183" s="2">
-        <v>1291.3612499999999</v>
-      </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>186</v>
-      </c>
-      <c r="B184" t="s">
-        <v>166</v>
-      </c>
-      <c r="C184" t="s">
-        <v>9</v>
-      </c>
-      <c r="D184" s="2">
-        <v>256</v>
-      </c>
-      <c r="E184" s="2">
-        <v>137.65004999999999</v>
-      </c>
-      <c r="F184" s="2">
-        <v>1203.25578</v>
-      </c>
-      <c r="G184" s="2">
         <v>1313.71325</v>
       </c>
     </row>

</xml_diff>